<commit_message>
move around some crack files
</commit_message>
<xml_diff>
--- a/crack_size_growth_v2.xlsx
+++ b/crack_size_growth_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\_fatigue3D_AM_imagebased_exp\fatigue_crack_tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Research\AM_fatigue\fatigue-crack-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590D87E6-2583-4502-A61A-7575F03E609D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610192A4-32D9-48C9-892D-EE13BFEBBB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMS2" sheetId="5" r:id="rId1"/>
@@ -19,12 +19,23 @@
     <sheet name="Green 5" sheetId="3" r:id="rId4"/>
     <sheet name="Green 6a" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t># cycle</t>
   </si>
@@ -50,18 +61,6 @@
   </si>
   <si>
     <t>#5_depth</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#11_area</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#11_side</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#11_depth</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -148,15 +147,57 @@
     <t>#9_depth</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>D, mm</t>
+  </si>
+  <si>
+    <t>a, mm</t>
+  </si>
+  <si>
+    <t>h, mm</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>#9</t>
+  </si>
+  <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>#11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,7 +228,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +239,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF7F"/>
         <bgColor rgb="FF00FF7F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -303,11 +350,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -336,6 +383,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -424,7 +474,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1701,7 +1751,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1212505199"/>
@@ -1763,7 +1813,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1212506031"/>
@@ -1805,7 +1855,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1842,7 +1892,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1918,7 +1968,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3195,7 +3245,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1223300687"/>
@@ -3257,7 +3307,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1223295695"/>
@@ -3299,7 +3349,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3336,7 +3386,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3412,7 +3462,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4689,7 +4739,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1418507759"/>
@@ -4751,7 +4801,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1418509839"/>
@@ -4793,7 +4843,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4830,7 +4880,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4906,7 +4956,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5112,7 +5162,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270617935"/>
@@ -5174,7 +5224,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270616687"/>
@@ -5222,7 +5272,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5306,7 +5356,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5512,7 +5562,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="361997263"/>
@@ -5574,7 +5624,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="361999343"/>
@@ -5622,7 +5672,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5698,7 +5748,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5904,7 +5954,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="364776127"/>
@@ -5966,7 +6016,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="364778207"/>
@@ -6014,7 +6064,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9884,391 +9934,518 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035D9A79-C5C3-4B01-9107-64EA0BCBB23E}">
-  <dimension ref="A2:Q12"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N16" sqref="N16"/>
+      <selection pane="topRight" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="9.19921875" customWidth="1"/>
-    <col min="3" max="3" width="9.69921875" customWidth="1"/>
-    <col min="4" max="4" width="9.8984375" customWidth="1"/>
-    <col min="17" max="17" width="9.19921875" customWidth="1"/>
+    <col min="2" max="2" width="9.25" customWidth="1"/>
+    <col min="3" max="3" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="10"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>9</v>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    <row r="5" spans="1:12">
+      <c r="A5" s="5">
         <v>0</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6">
-        <v>0</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <f>SQRT(J3)</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="6">
-        <v>0</v>
-      </c>
-      <c r="P3" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>20000</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <f t="shared" ref="M4:M12" si="0">SQRT(J4)</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="6">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>50000</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="J5" s="6">
-        <v>1.1333333333333332E-2</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0.20299999999999999</v>
-      </c>
-      <c r="L5" s="6">
-        <v>5.4999999999999993E-2</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="0"/>
-        <v>0.1064581294844754</v>
-      </c>
-      <c r="O5" s="6">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>0</v>
-      </c>
+      <c r="I5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="5">
-        <v>80000</v>
+        <v>20000</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="J6" s="6">
-        <v>0.43733333333333335</v>
-      </c>
-      <c r="K6" s="6">
-        <v>2.0363333333333333</v>
-      </c>
-      <c r="L6" s="6">
-        <v>0.35466666666666669</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="0"/>
-        <v>0.66131182760731977</v>
-      </c>
-      <c r="O6" s="6">
-        <v>5.1666666666666666E-2</v>
-      </c>
-      <c r="P6" s="6">
-        <v>0.3136666666666667</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>0.16133333333333333</v>
-      </c>
+      <c r="I6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="5">
-        <v>90000</v>
+        <v>50000</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="J7" s="6">
-        <v>0.68366666666666676</v>
-      </c>
-      <c r="K7" s="6">
-        <v>2.1313333333333335</v>
-      </c>
-      <c r="L7" s="6">
-        <v>0.41366666666666668</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="0"/>
-        <v>0.82684137938704227</v>
-      </c>
-      <c r="O7" s="6">
-        <v>8.3666666666666667E-2</v>
-      </c>
-      <c r="P7" s="6">
-        <v>0.48166666666666663</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>0.18733333333333335</v>
-      </c>
+      <c r="I7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="5">
-        <v>91000</v>
+        <v>80000</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="J8" s="6">
-        <v>0.72966666666666669</v>
-      </c>
-      <c r="K8" s="6">
-        <v>2.3119999999999998</v>
-      </c>
-      <c r="L8" s="6">
-        <v>0.45333333333333337</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="0"/>
-        <v>0.85420528367990478</v>
-      </c>
-      <c r="O8" s="6">
-        <v>9.7333333333333341E-2</v>
-      </c>
-      <c r="P8" s="6">
-        <v>0.49899999999999994</v>
-      </c>
-      <c r="Q8" s="6">
-        <v>0.222</v>
-      </c>
+      <c r="I8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="5">
-        <v>92000</v>
+        <v>90000</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="J9" s="6">
-        <v>0.77966666666666662</v>
-      </c>
-      <c r="K9" s="6">
-        <v>2.4263333333333335</v>
-      </c>
-      <c r="L9" s="6">
-        <v>0.47799999999999998</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="0"/>
-        <v>0.88298735362782321</v>
-      </c>
-      <c r="O9" s="6">
-        <v>0.10466666666666667</v>
-      </c>
-      <c r="P9" s="6">
-        <v>0.60966666666666658</v>
-      </c>
-      <c r="Q9" s="6">
-        <v>0.22166666666666668</v>
-      </c>
+      <c r="I9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="5">
-        <v>95000</v>
+        <v>91000</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="J10" s="6">
-        <v>0.94266666666666665</v>
-      </c>
-      <c r="K10" s="6">
-        <v>2.7869999999999995</v>
-      </c>
-      <c r="L10" s="6">
-        <v>0.5093333333333333</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="0"/>
-        <v>0.97091022585338271</v>
-      </c>
-      <c r="O10" s="6">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="P10" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>0.25333333333333335</v>
-      </c>
+      <c r="I10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="5">
-        <v>100000</v>
+        <v>92000</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="J11" s="6">
-        <v>1.3273333333333333</v>
-      </c>
-      <c r="K11" s="6">
-        <v>2.8290000000000002</v>
-      </c>
-      <c r="L11" s="6">
-        <v>0.68166666666666664</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="0"/>
-        <v>1.1520995327372254</v>
-      </c>
-      <c r="O11" s="6">
-        <v>0.16866666666666666</v>
-      </c>
-      <c r="P11" s="6">
-        <v>0.71599999999999986</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>0.30166666666666669</v>
-      </c>
+      <c r="I11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="5">
-        <v>105000</v>
+        <v>95000</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="J12" s="6">
-        <v>2.0340000000000003</v>
-      </c>
-      <c r="K12" s="6">
-        <v>3.7226666666666666</v>
-      </c>
-      <c r="L12" s="6">
-        <v>0.81133333333333335</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="0"/>
-        <v>1.4261837188805657</v>
-      </c>
-      <c r="O12" s="6">
-        <v>0.17533333333333334</v>
-      </c>
-      <c r="P12" s="6">
-        <v>0.71866666666666668</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>0.34333333333333332</v>
-      </c>
+      <c r="I12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="5">
+        <v>100000</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="5">
+        <v>105000</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="5">
+        <v>0</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="5">
+        <v>50000</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="5">
+        <v>80000</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="5">
+        <v>90000</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="5">
+        <v>91000</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="5">
+        <v>92000</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="5">
+        <v>95000</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="5">
+        <v>100000</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="5">
+        <v>105000</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="5">
+        <v>0</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="5">
+        <v>50000</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="5">
+        <v>80000</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="5">
+        <v>90000</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="5">
+        <v>91000</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="5">
+        <v>92000</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="5">
+        <v>95000</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="5">
+        <v>100000</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="5">
+        <v>105000</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -10285,22 +10462,22 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="10.69921875" customWidth="1"/>
-    <col min="3" max="3" width="9.19921875" customWidth="1"/>
-    <col min="4" max="4" width="8.19921875" customWidth="1"/>
+    <col min="1" max="2" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="9.25" customWidth="1"/>
+    <col min="4" max="4" width="8.25" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="9.69921875" customWidth="1"/>
-    <col min="7" max="7" width="10.69921875" customWidth="1"/>
-    <col min="8" max="8" width="13.59765625" customWidth="1"/>
-    <col min="9" max="10" width="10.19921875" customWidth="1"/>
-    <col min="11" max="11" width="10.59765625" customWidth="1"/>
-    <col min="12" max="12" width="11.69921875" customWidth="1"/>
-    <col min="13" max="13" width="10.19921875" customWidth="1"/>
-    <col min="14" max="14" width="11.3984375" customWidth="1"/>
+    <col min="6" max="6" width="9.75" customWidth="1"/>
+    <col min="7" max="7" width="10.75" customWidth="1"/>
+    <col min="8" max="8" width="13.625" customWidth="1"/>
+    <col min="9" max="10" width="10.25" customWidth="1"/>
+    <col min="11" max="11" width="10.625" customWidth="1"/>
+    <col min="12" max="12" width="11.75" customWidth="1"/>
+    <col min="13" max="13" width="10.25" customWidth="1"/>
+    <col min="14" max="14" width="11.375" customWidth="1"/>
     <col min="15" max="15" width="9.5" customWidth="1"/>
-    <col min="16" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="16" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -10320,11 +10497,11 @@
       <selection sqref="A1:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="16" width="10.69921875" customWidth="1"/>
-    <col min="17" max="17" width="12.19921875" customWidth="1"/>
-    <col min="18" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="1" max="16" width="10.75" customWidth="1"/>
+    <col min="17" max="17" width="12.25" customWidth="1"/>
+    <col min="18" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -10344,13 +10521,13 @@
       <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="26" width="10.69921875" customWidth="1"/>
-    <col min="32" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="1" max="26" width="10.75" customWidth="1"/>
+    <col min="32" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -10367,13 +10544,13 @@
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>0</v>
@@ -10391,28 +10568,28 @@
         <v>0</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="A3">
         <v>80000</v>
       </c>
@@ -10438,7 +10615,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24">
       <c r="A4">
         <v>90000</v>
       </c>
@@ -10464,7 +10641,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="A5">
         <v>100000</v>
       </c>
@@ -10490,7 +10667,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24">
       <c r="A6">
         <v>105000</v>
       </c>
@@ -10516,7 +10693,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="A7">
         <v>115000</v>
       </c>
@@ -10542,7 +10719,7 @@
         <v>115000</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="A8">
         <v>125000</v>
       </c>
@@ -10568,7 +10745,7 @@
         <v>125000</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24">
       <c r="A9">
         <v>135000</v>
       </c>
@@ -10603,7 +10780,7 @@
         <v>135000</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24">
       <c r="A10">
         <v>145000</v>
       </c>
@@ -10638,7 +10815,7 @@
         <v>145000</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24">
       <c r="A11">
         <v>155000</v>
       </c>
@@ -10682,7 +10859,7 @@
         <v>3.92469713729365E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24">
       <c r="A12">
         <v>175000</v>
       </c>
@@ -10735,7 +10912,7 @@
         <v>5.0838484916259502E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="A13">
         <v>195000</v>
       </c>
@@ -10788,7 +10965,7 @@
         <v>0.12621611691672899</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24">
       <c r="A14">
         <v>215000</v>
       </c>
@@ -10850,7 +11027,7 @@
         <v>5.14299852570844E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24">
       <c r="A15">
         <v>225000</v>
       </c>
@@ -10912,7 +11089,7 @@
         <v>0.11391790821570499</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24">
       <c r="A16">
         <v>235000</v>
       </c>
@@ -10974,7 +11151,7 @@
         <v>6.5728018841552396E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24">
       <c r="A17">
         <v>245000</v>
       </c>
@@ -11036,57 +11213,57 @@
         <v>6.4449969207186694E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24">
       <c r="A22">
         <v>80000</v>
       </c>
@@ -11100,7 +11277,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24">
       <c r="A23">
         <v>90000</v>
       </c>
@@ -11114,7 +11291,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24">
       <c r="A24">
         <v>100000</v>
       </c>
@@ -11128,7 +11305,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24">
       <c r="A25">
         <v>105000</v>
       </c>
@@ -11142,7 +11319,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24">
       <c r="A26">
         <v>115000</v>
       </c>
@@ -11156,7 +11333,7 @@
         <v>115000</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24">
       <c r="A27">
         <v>125000</v>
       </c>
@@ -11170,7 +11347,7 @@
         <v>125000</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24">
       <c r="A28">
         <v>135000</v>
       </c>
@@ -11202,7 +11379,7 @@
         <v>0.28842538296747899</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24">
       <c r="A29">
         <v>145000</v>
       </c>
@@ -11234,7 +11411,7 @@
         <v>0.24612916781514799</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24">
       <c r="A30">
         <v>155000</v>
       </c>
@@ -11266,7 +11443,7 @@
         <v>0.41710503614362299</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24">
       <c r="A31">
         <v>175000</v>
       </c>
@@ -11307,7 +11484,7 @@
         <v>0.48465204324982197</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24">
       <c r="A32">
         <v>195000</v>
       </c>
@@ -11357,7 +11534,7 @@
         <v>0.550969778547587</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19">
       <c r="A33">
         <v>215000</v>
       </c>
@@ -11407,7 +11584,7 @@
         <v>1.0405666476426001</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19">
       <c r="A34">
         <v>225000</v>
       </c>
@@ -11457,7 +11634,7 @@
         <v>1.3650029220936299</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19">
       <c r="A35">
         <v>235000</v>
       </c>
@@ -11507,7 +11684,7 @@
         <v>1.5028270584451799</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19">
       <c r="A36">
         <v>245000</v>
       </c>
@@ -11577,14 +11754,14 @@
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="6" width="10.69921875" customWidth="1"/>
-    <col min="7" max="7" width="21.09765625" customWidth="1"/>
-    <col min="8" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="1" max="6" width="10.75" customWidth="1"/>
+    <col min="7" max="7" width="21.125" customWidth="1"/>
+    <col min="8" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -11598,7 +11775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7">
         <v>0</v>
       </c>
@@ -11612,7 +11789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="9">
         <v>50000</v>
       </c>
@@ -11626,7 +11803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="9">
         <v>80000</v>
       </c>
@@ -11640,7 +11817,7 @@
         <v>0.32737261126886702</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="9">
         <v>90000</v>
       </c>
@@ -11654,7 +11831,7 @@
         <v>0.38087620029045899</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="9">
         <v>100000</v>
       </c>
@@ -11668,7 +11845,7 @@
         <v>0.538358137185728</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="9">
         <v>105000</v>
       </c>
@@ -11682,7 +11859,7 @@
         <v>0.78349716215379905</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="9">
         <v>115000</v>
       </c>
@@ -11696,7 +11873,7 @@
         <v>0.88688775258833297</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="9">
         <v>125000</v>
       </c>
@@ -11710,7 +11887,7 @@
         <v>0.92712200436315095</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="9">
         <v>130000</v>
       </c>
@@ -11724,7 +11901,7 @@
         <v>1.0912931643039201</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="9">
         <v>135000</v>
       </c>
@@ -11738,7 +11915,7 @@
         <v>1.22791836952805</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="9">
         <v>140000</v>
       </c>
@@ -11752,7 +11929,7 @@
         <v>1.3904708287126399</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="9">
         <v>150000</v>
       </c>
@@ -11766,7 +11943,7 @@
         <v>1.9770436700256999</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="9">
         <v>160000</v>
       </c>
@@ -11780,46 +11957,46 @@
         <v>3.4835405999620601</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
measured the geometric info of AMS2
</commit_message>
<xml_diff>
--- a/crack_size_growth_v2.xlsx
+++ b/crack_size_growth_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Research\AM_fatigue\fatigue-crack-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610192A4-32D9-48C9-892D-EE13BFEBBB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCC6A3E-D28A-4B47-8E49-374836100E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMS2" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t># cycle</t>
   </si>
@@ -151,15 +151,6 @@
     <t>#1</t>
   </si>
   <si>
-    <t>D, mm</t>
-  </si>
-  <si>
-    <t>a, mm</t>
-  </si>
-  <si>
-    <t>h, mm</t>
-  </si>
-  <si>
     <t>#2</t>
   </si>
   <si>
@@ -188,6 +179,18 @@
   </si>
   <si>
     <t>#11</t>
+  </si>
+  <si>
+    <t>Pixel</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -385,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -9934,11 +9937,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035D9A79-C5C3-4B01-9107-64EA0BCBB23E}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G42" sqref="G42"/>
+      <selection pane="topRight" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9949,73 +9952,70 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="B1" s="10">
+        <v>552</v>
+      </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="10">
+        <v>6.1000000000000004E-3</v>
+      </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="K4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="5">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="5">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -10028,7 +10028,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="5">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -10041,7 +10041,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="5">
-        <v>80000</v>
+        <v>50000</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -10054,12 +10054,20 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="5">
-        <v>90000</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+        <v>80000</v>
+      </c>
+      <c r="B9" s="6">
+        <v>24</v>
+      </c>
+      <c r="C9" s="6">
+        <v>78</v>
+      </c>
+      <c r="E9" s="6">
+        <v>23</v>
+      </c>
+      <c r="F9" s="6">
+        <v>102</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="K9" s="6"/>
@@ -10067,12 +10075,20 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="5">
-        <v>91000</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+        <v>90000</v>
+      </c>
+      <c r="B10" s="6">
+        <v>29</v>
+      </c>
+      <c r="C10" s="6">
+        <v>88</v>
+      </c>
+      <c r="E10" s="6">
+        <v>26</v>
+      </c>
+      <c r="F10" s="6">
+        <v>104</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="K10" s="6"/>
@@ -10080,12 +10096,20 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5">
-        <v>92000</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+        <v>91000</v>
+      </c>
+      <c r="B11" s="6">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6">
+        <v>90</v>
+      </c>
+      <c r="E11" s="6">
+        <v>34</v>
+      </c>
+      <c r="F11" s="6">
+        <v>112</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="K11" s="6"/>
@@ -10093,12 +10117,20 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="5">
-        <v>95000</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+        <v>92000</v>
+      </c>
+      <c r="B12" s="6">
+        <v>30</v>
+      </c>
+      <c r="C12" s="6">
+        <v>92</v>
+      </c>
+      <c r="E12" s="6">
+        <v>36</v>
+      </c>
+      <c r="F12" s="6">
+        <v>116</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="K12" s="6"/>
@@ -10106,89 +10138,133 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="5">
-        <v>100000</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+        <v>95000</v>
+      </c>
+      <c r="B13" s="6">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6">
+        <v>92</v>
+      </c>
+      <c r="E13" s="6">
+        <v>37</v>
+      </c>
+      <c r="F13" s="6">
+        <v>120</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+      <c r="K13" s="6">
+        <v>10</v>
+      </c>
+      <c r="L13" s="6">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="5">
+        <v>100000</v>
+      </c>
+      <c r="B14" s="6">
+        <v>32</v>
+      </c>
+      <c r="C14" s="6">
+        <v>100</v>
+      </c>
+      <c r="E14" s="6">
+        <v>37</v>
+      </c>
+      <c r="F14" s="6">
+        <v>120</v>
+      </c>
+      <c r="H14" s="6">
+        <v>20</v>
+      </c>
+      <c r="I14" s="6">
+        <v>42</v>
+      </c>
+      <c r="K14" s="6">
+        <v>13</v>
+      </c>
+      <c r="L14" s="6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="5">
         <v>105000</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" t="s">
-        <v>38</v>
+      <c r="B15" s="6">
+        <v>32</v>
+      </c>
+      <c r="C15" s="6">
+        <v>102</v>
+      </c>
+      <c r="E15" s="6">
+        <v>40</v>
+      </c>
+      <c r="F15" s="6">
+        <v>128</v>
+      </c>
+      <c r="H15" s="6">
+        <v>27</v>
+      </c>
+      <c r="I15" s="6">
+        <v>76</v>
+      </c>
+      <c r="K15" s="6">
+        <v>17</v>
+      </c>
+      <c r="L15" s="6">
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>31</v>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="5">
+      <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="5">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -10201,7 +10277,7 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="5">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -10214,10 +10290,14 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="5">
-        <v>80000</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+        <v>50000</v>
+      </c>
+      <c r="B22" s="6">
+        <v>10</v>
+      </c>
+      <c r="C22" s="6">
+        <v>60</v>
+      </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="H22" s="6"/>
@@ -10227,12 +10307,20 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="5">
-        <v>90000</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+        <v>80000</v>
+      </c>
+      <c r="B23" s="6">
+        <v>46</v>
+      </c>
+      <c r="C23" s="6">
+        <v>280</v>
+      </c>
+      <c r="E23" s="6">
+        <v>24</v>
+      </c>
+      <c r="F23" s="6">
+        <v>66</v>
+      </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="K23" s="6"/>
@@ -10240,117 +10328,203 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="5">
-        <v>91000</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+        <v>90000</v>
+      </c>
+      <c r="B24" s="6">
+        <v>65</v>
+      </c>
+      <c r="C24" s="6">
+        <v>328</v>
+      </c>
+      <c r="E24" s="6">
+        <v>30</v>
+      </c>
+      <c r="F24" s="6">
+        <v>104</v>
+      </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
+      <c r="K24" s="6">
+        <v>18</v>
+      </c>
+      <c r="L24" s="6">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="5">
-        <v>92000</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+        <v>91000</v>
+      </c>
+      <c r="B25" s="6">
+        <v>70</v>
+      </c>
+      <c r="C25" s="6">
+        <v>328</v>
+      </c>
+      <c r="E25" s="6">
+        <v>30</v>
+      </c>
+      <c r="F25" s="6">
+        <v>106</v>
+      </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
+      <c r="K25" s="6">
+        <v>18</v>
+      </c>
+      <c r="L25" s="6">
+        <v>58</v>
+      </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="5">
-        <v>95000</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+        <v>92000</v>
+      </c>
+      <c r="B26" s="6">
+        <v>72</v>
+      </c>
+      <c r="C26" s="6">
+        <v>332</v>
+      </c>
+      <c r="E26" s="6">
+        <v>33</v>
+      </c>
+      <c r="F26" s="6">
+        <v>106</v>
+      </c>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
+      <c r="K26" s="6">
+        <v>19</v>
+      </c>
+      <c r="L26" s="6">
+        <v>59</v>
+      </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="5">
-        <v>100000</v>
-      </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
+        <v>95000</v>
+      </c>
+      <c r="B27" s="6">
+        <v>88</v>
+      </c>
+      <c r="C27" s="6">
+        <v>360</v>
+      </c>
+      <c r="E27" s="6">
+        <v>38</v>
+      </c>
+      <c r="F27" s="6">
+        <v>110</v>
+      </c>
+      <c r="H27" s="6">
+        <v>22</v>
+      </c>
+      <c r="I27" s="6">
+        <v>64</v>
+      </c>
+      <c r="K27" s="6">
+        <v>26</v>
+      </c>
+      <c r="L27" s="6">
+        <v>61</v>
+      </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="5">
+        <v>100000</v>
+      </c>
+      <c r="B28" s="6">
+        <v>120</v>
+      </c>
+      <c r="C28" s="6">
+        <v>400</v>
+      </c>
+      <c r="E28" s="6">
+        <v>51</v>
+      </c>
+      <c r="F28" s="6">
+        <v>162</v>
+      </c>
+      <c r="H28" s="6">
+        <v>29</v>
+      </c>
+      <c r="I28" s="6">
+        <v>86</v>
+      </c>
+      <c r="K28" s="6">
+        <v>26</v>
+      </c>
+      <c r="L28" s="6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="5">
         <v>105000</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="B31" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" t="s">
-        <v>40</v>
-      </c>
-      <c r="H31" t="s">
-        <v>41</v>
+      <c r="B29" s="6">
+        <v>146</v>
+      </c>
+      <c r="C29" s="6">
+        <v>460</v>
+      </c>
+      <c r="E29" s="6">
+        <v>64</v>
+      </c>
+      <c r="F29" s="6">
+        <v>192</v>
+      </c>
+      <c r="H29" s="6">
+        <v>38</v>
+      </c>
+      <c r="I29" s="6">
+        <v>120</v>
+      </c>
+      <c r="K29" s="6">
+        <v>32</v>
+      </c>
+      <c r="L29" s="6">
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>31</v>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="5">
+      <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+      <c r="B33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="5">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -10361,7 +10535,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="5">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -10372,7 +10546,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="5">
-        <v>80000</v>
+        <v>50000</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -10383,69 +10557,160 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="5">
-        <v>90000</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
+        <v>80000</v>
+      </c>
+      <c r="B37" s="6">
+        <v>21</v>
+      </c>
+      <c r="C37" s="6">
+        <v>52</v>
+      </c>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
+      <c r="H37" s="6">
+        <v>28</v>
+      </c>
+      <c r="I37" s="6">
+        <v>66</v>
+      </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="5">
-        <v>91000</v>
-      </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
+        <v>90000</v>
+      </c>
+      <c r="B38" s="6">
+        <v>26</v>
+      </c>
+      <c r="C38" s="6">
+        <v>70</v>
+      </c>
+      <c r="E38" s="6">
+        <v>28</v>
+      </c>
+      <c r="F38" s="6">
+        <v>64</v>
+      </c>
+      <c r="H38" s="6">
+        <v>37</v>
+      </c>
+      <c r="I38" s="6">
+        <v>79</v>
+      </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="5">
-        <v>92000</v>
-      </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
+        <v>91000</v>
+      </c>
+      <c r="B39" s="6">
+        <v>26</v>
+      </c>
+      <c r="C39" s="6">
+        <v>70</v>
+      </c>
+      <c r="E39" s="6">
+        <v>28</v>
+      </c>
+      <c r="F39" s="6">
+        <v>64</v>
+      </c>
+      <c r="H39" s="6">
+        <v>38</v>
+      </c>
+      <c r="I39" s="6">
+        <v>99</v>
+      </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="5">
-        <v>95000</v>
-      </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
+        <v>92000</v>
+      </c>
+      <c r="B40" s="6">
+        <v>28</v>
+      </c>
+      <c r="C40" s="6">
+        <v>71</v>
+      </c>
+      <c r="E40" s="6">
+        <v>28</v>
+      </c>
+      <c r="F40" s="6">
+        <v>76</v>
+      </c>
+      <c r="H40" s="6">
+        <v>46</v>
+      </c>
+      <c r="I40" s="6">
+        <v>106</v>
+      </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="5">
-        <v>100000</v>
-      </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
+        <v>95000</v>
+      </c>
+      <c r="B41" s="6">
+        <v>35</v>
+      </c>
+      <c r="C41" s="6">
+        <v>78</v>
+      </c>
+      <c r="E41" s="6">
+        <v>32</v>
+      </c>
+      <c r="F41" s="6">
+        <v>78</v>
+      </c>
+      <c r="H41" s="6">
+        <v>50</v>
+      </c>
+      <c r="I41" s="6">
+        <v>110</v>
+      </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="5">
+        <v>100000</v>
+      </c>
+      <c r="B42" s="6">
+        <v>36</v>
+      </c>
+      <c r="C42" s="6">
+        <v>82</v>
+      </c>
+      <c r="E42" s="6">
+        <v>37</v>
+      </c>
+      <c r="F42" s="6">
+        <v>85</v>
+      </c>
+      <c r="H42" s="6">
+        <v>50</v>
+      </c>
+      <c r="I42" s="6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="5">
         <v>105000</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
+      <c r="B43" s="6">
+        <v>38</v>
+      </c>
+      <c r="C43" s="6">
+        <v>90</v>
+      </c>
+      <c r="E43" s="6">
+        <v>39</v>
+      </c>
+      <c r="F43" s="6">
+        <v>86</v>
+      </c>
+      <c r="H43" s="6">
+        <v>58</v>
+      </c>
+      <c r="I43" s="6">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
computed the dadN-dK curve for sample G6a
</commit_message>
<xml_diff>
--- a/crack_size_growth_v2.xlsx
+++ b/crack_size_growth_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\_fatigue3D_AM_imagebased_exp\fatigue_crack_tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D15022-8443-4A9E-AA01-E0F5397AB065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC0CF09-5EBA-4C25-BF60-B728A40C5744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ref_Cao 2018" sheetId="6" r:id="rId1"/>
@@ -4185,7 +4185,17 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20137343675586231"/>
+          <c:y val="0.10478805423662284"/>
+          <c:w val="0.20323381964612247"/>
+          <c:h val="0.63471882266921598"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -26680,15 +26690,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>364435</xdr:colOff>
+      <xdr:colOff>351182</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>24848</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>521805</xdr:colOff>
+      <xdr:colOff>508552</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>99390</xdr:rowOff>
+      <xdr:rowOff>74543</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -27245,8 +27255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244E426E-687C-4E0B-8132-6FA78000E5B9}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -27590,9 +27600,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035D9A79-C5C3-4B01-9107-64EA0BCBB23E}">
   <dimension ref="A1:T137"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD31" sqref="AD31"/>
+      <selection pane="topRight" activeCell="L72" sqref="L72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -33967,8 +33977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added the small crack growth data
</commit_message>
<xml_diff>
--- a/crack_size_growth_v2.xlsx
+++ b/crack_size_growth_v2.xlsx
@@ -5,27 +5,38 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\_fatigue3D_AM_imagebased_exp\fatigue_crack_tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Research\AM_fatigue\fatigue-crack-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC0CF09-5EBA-4C25-BF60-B728A40C5744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835E44BF-E018-429E-9095-4C219C7DDB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ref_Cao 2018" sheetId="6" r:id="rId1"/>
+    <sheet name="Ref_dadN-dK" sheetId="6" r:id="rId1"/>
     <sheet name="AMS2" sheetId="5" r:id="rId2"/>
     <sheet name="Yellow 6" sheetId="1" r:id="rId3"/>
     <sheet name="Yellow 6a" sheetId="2" r:id="rId4"/>
     <sheet name="Green 5" sheetId="3" r:id="rId5"/>
     <sheet name="Green 6a" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="65">
   <si>
     <t># cycle</t>
   </si>
@@ -238,17 +249,29 @@
   <si>
     <t>Straight line region</t>
   </si>
+  <si>
+    <t>Fei Cao, 2018, Jom</t>
+  </si>
+  <si>
+    <t>da/dN, mm/cycle</t>
+  </si>
+  <si>
+    <t>Fei Cao, 2018, Jom, Total</t>
+  </si>
+  <si>
+    <t>Caton et al., IJF, 2012</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
-    <numFmt numFmtId="177" formatCode="0.00000"/>
-    <numFmt numFmtId="178" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +304,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -408,11 +438,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -443,10 +473,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -460,6 +490,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -505,6 +538,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ref_dadN-dK'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fei Cao, 2018, Jom</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -543,8 +587,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.4541330605367106E-2"/>
-                  <c:y val="1.0090755004398292E-2"/>
+                  <c:x val="5.6398650105623435E-2"/>
+                  <c:y val="-7.6224069682303164E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="0.0000E+00" sourceLinked="0"/>
@@ -560,7 +604,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -572,14 +616,14 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ref_Cao 2018'!$B$12:$B$28</c:f>
+              <c:f>'Ref_dadN-dK'!$B$13:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -639,7 +683,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ref_Cao 2018'!$C$12:$C$28</c:f>
+              <c:f>'Ref_dadN-dK'!$C$13:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="17"/>
@@ -707,6 +751,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ref_dadN-dK'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fei Cao, 2018, Jom, Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -731,7 +786,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ref_Cao 2018'!$B$4:$B$39</c:f>
+              <c:f>'Ref_dadN-dK'!$B$5:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -848,7 +903,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ref_Cao 2018'!$C$4:$C$39</c:f>
+              <c:f>'Ref_dadN-dK'!$C$5:$C$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="36"/>
@@ -967,6 +1022,165 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-EB6F-4860-9FEA-7ADB0C428558}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ref_dadN-dK'!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Caton et al., IJF, 2012</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.6362626057982242E-2"/>
+                  <c:y val="5.0170848085315196E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.0000E+00" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ref_dadN-dK'!$H$5:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.37711773893842199</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6985787449816</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2542509082599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8967946188090099</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7159832795544299</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0122435917289696</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.7002656958327602</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.7281953503475203</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ref_dadN-dK'!$J$5:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.5423123535160999E-11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5465300835993599E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1714820722636105E-10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1222206276760299E-9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2254499953910903E-9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7430350939300298E-9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.5768052809248291E-9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7045584328470601E-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C522-47B3-A04F-1086B45C3B65}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1068,7 +1282,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="zh-CN"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1106,7 +1320,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="438476079"/>
@@ -1201,14 +1415,14 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="zh-CN"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1239,7 +1453,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="438464015"/>
@@ -1254,6 +1468,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.69894262423525977"/>
+          <c:y val="0.58578339102892529"/>
+          <c:w val="0.30105737576474029"/>
+          <c:h val="0.27573715307056945"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1287,7 +1542,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1399,7 +1654,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1522,7 +1777,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1631,7 +1886,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="913201456"/>
@@ -1693,7 +1948,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="913204368"/>
@@ -1735,7 +1990,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1772,7 +2027,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1884,7 +2139,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2007,7 +2262,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2122,7 +2377,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="621951696"/>
@@ -2184,7 +2439,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="621939216"/>
@@ -2226,7 +2481,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2263,7 +2518,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2375,7 +2630,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2498,7 +2753,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2613,7 +2868,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="872659904"/>
@@ -2675,7 +2930,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="872658656"/>
@@ -2717,7 +2972,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2754,7 +3009,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3224,7 +3479,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3895,6 +4150,171 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000B-01AA-429D-AEFA-06580E72687B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ref_dadN-dK'!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Caton et al., IJF, 2012</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.13394087129540086"/>
+                  <c:y val="0.31055010195819144"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ref_dadN-dK'!$H$5:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.37711773893842199</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6985787449816</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2542509082599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8967946188090099</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7159832795544299</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0122435917289696</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.7002656958327602</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.7281953503475203</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ref_dadN-dK'!$J$5:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.5423123535160999E-11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5465300835993599E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1714820722636105E-10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1222206276760299E-9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2254499953910903E-9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7430350939300298E-9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.5768052809248291E-9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7045584328470601E-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FE06-41E5-842F-D8A881005388}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3997,7 +4417,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="zh-CN"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4035,7 +4455,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="347676607"/>
@@ -4130,7 +4550,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="zh-CN"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4168,7 +4588,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="356877151"/>
@@ -4189,10 +4609,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.20137343675586231"/>
-          <c:y val="0.10478805423662284"/>
-          <c:w val="0.20323381964612247"/>
-          <c:h val="0.63471882266921598"/>
+          <c:x val="5.3151321463483933E-2"/>
+          <c:y val="5.1580866138073556E-2"/>
+          <c:w val="0.30279525415297831"/>
+          <c:h val="0.89521196411010728"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -4220,7 +4640,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4257,7 +4677,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4830,7 +5250,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5499,7 +5919,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="zh-CN"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5537,7 +5957,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="343169423"/>
@@ -5632,7 +6052,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="zh-CN"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5670,7 +6090,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="343159855"/>
@@ -5712,7 +6132,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5749,7 +6169,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5825,7 +6245,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7102,7 +7522,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1212505199"/>
@@ -7164,7 +7584,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1212506031"/>
@@ -7206,7 +7626,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7243,7 +7663,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7319,7 +7739,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8596,7 +9016,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1223300687"/>
@@ -8658,7 +9078,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1223295695"/>
@@ -8700,7 +9120,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -8737,7 +9157,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8813,7 +9233,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -10090,7 +10510,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1418507759"/>
@@ -10152,7 +10572,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1418509839"/>
@@ -10194,7 +10614,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -10231,7 +10651,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10343,7 +10763,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -10520,7 +10940,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -10682,7 +11102,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="809502976"/>
@@ -10744,7 +11164,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="809501312"/>
@@ -10792,7 +11212,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10904,7 +11324,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -11099,7 +11519,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="zh-CN"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11137,7 +11557,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="347676607"/>
@@ -11232,7 +11652,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="zh-CN"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11270,7 +11690,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="356877151"/>
@@ -11312,7 +11732,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -11349,7 +11769,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11461,7 +11881,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -11614,7 +12034,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -11752,7 +12172,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="630899168"/>
@@ -11814,7 +12234,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="623306048"/>
@@ -11856,7 +12276,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -11893,7 +12313,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -12005,7 +12425,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -12152,7 +12572,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -12290,7 +12710,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="721987040"/>
@@ -12352,7 +12772,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="721985376"/>
@@ -12394,7 +12814,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -12431,7 +12851,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -12543,7 +12963,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -12704,7 +13124,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -12842,7 +13262,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="809502976"/>
@@ -12904,7 +13324,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="809501312"/>
@@ -12950,7 +13370,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -12987,7 +13407,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -13099,7 +13519,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -13252,7 +13672,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -13390,7 +13810,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="881369744"/>
@@ -13452,7 +13872,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="881375152"/>
@@ -13494,7 +13914,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -13531,7 +13951,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -13643,7 +14063,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -13784,7 +14204,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -13917,7 +14337,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="881607376"/>
@@ -13979,7 +14399,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="881606544"/>
@@ -14021,7 +14441,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -14058,7 +14478,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -14170,7 +14590,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -14323,7 +14743,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -14461,7 +14881,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="874130000"/>
@@ -14523,7 +14943,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="874134576"/>
@@ -14565,7 +14985,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -14602,7 +15022,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -14714,7 +15134,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -14861,7 +15281,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -14994,7 +15414,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="901136224"/>
@@ -15056,7 +15476,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="901139552"/>
@@ -15098,7 +15518,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -15135,7 +15555,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -15247,7 +15667,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -15394,7 +15814,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -15532,7 +15952,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="904732848"/>
@@ -15594,7 +16014,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="904724944"/>
@@ -15636,7 +16056,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -15673,7 +16093,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -26252,16 +26672,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>52385</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>223836</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>676274</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -27253,341 +27673,442 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244E426E-687C-4E0B-8132-6FA78000E5B9}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I13" sqref="I13:K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="17.69921875" customWidth="1"/>
-    <col min="3" max="3" width="14.69921875" customWidth="1"/>
+    <col min="2" max="2" width="17.75" customWidth="1"/>
+    <col min="3" max="3" width="14.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:10" s="16" customFormat="1" ht="20.25">
+      <c r="A1" s="16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="16" customFormat="1" ht="20.25"/>
+    <row r="3" spans="1:10">
       <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" t="s">
         <v>59</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>55</v>
       </c>
+      <c r="H4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="5" spans="1:10">
+      <c r="B5">
         <v>3.03488931872231</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C5" s="12">
         <v>5.9355387543338298E-11</v>
       </c>
+      <c r="H5">
+        <v>0.37711773893842199</v>
+      </c>
+      <c r="I5" s="12">
+        <v>4.5423123535161E-8</v>
+      </c>
+      <c r="J5" s="12">
+        <f>I5*0.001</f>
+        <v>4.5423123535160999E-11</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5">
+    <row r="6" spans="1:10">
+      <c r="B6">
         <v>3.0662470462727298</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C6" s="12">
         <v>1.03982690578927E-10</v>
       </c>
+      <c r="H6">
+        <v>0.6985787449816</v>
+      </c>
+      <c r="I6" s="12">
+        <v>1.5465300835993599E-7</v>
+      </c>
+      <c r="J6" s="12">
+        <f t="shared" ref="J6:J12" si="0">I6*0.001</f>
+        <v>1.5465300835993599E-10</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6">
+    <row r="7" spans="1:10">
+      <c r="B7">
         <v>3.1299378519892298</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C7" s="12">
         <v>1.44223265986385E-10</v>
       </c>
+      <c r="H7">
+        <v>1.2542509082599</v>
+      </c>
+      <c r="I7" s="12">
+        <v>5.1714820722636103E-7</v>
+      </c>
+      <c r="J7" s="12">
+        <f t="shared" si="0"/>
+        <v>5.1714820722636105E-10</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7">
+    <row r="8" spans="1:10">
+      <c r="B8">
         <v>3.2613158199877499</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C8" s="12">
         <v>2.00057524839119E-10</v>
       </c>
+      <c r="H8">
+        <v>1.8967946188090099</v>
+      </c>
+      <c r="I8">
+        <v>1.1222206276760299E-6</v>
+      </c>
+      <c r="J8" s="12">
+        <f t="shared" si="0"/>
+        <v>1.1222206276760299E-9</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="9" spans="1:10">
+      <c r="B9">
         <v>3.4333200182819898</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C9" s="12">
         <v>2.97667818069626E-10</v>
       </c>
+      <c r="H9">
+        <v>2.7159832795544299</v>
+      </c>
+      <c r="I9">
+        <v>2.22544999539109E-6</v>
+      </c>
+      <c r="J9" s="12">
+        <f t="shared" si="0"/>
+        <v>2.2254499953910903E-9</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9">
+    <row r="10" spans="1:10">
+      <c r="B10">
         <v>3.65174127254837</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C10" s="12">
         <v>4.8630779609571999E-10</v>
       </c>
+      <c r="H10">
+        <v>4.0122435917289696</v>
+      </c>
+      <c r="I10">
+        <v>4.7430350939300298E-6</v>
+      </c>
+      <c r="J10" s="12">
+        <f t="shared" si="0"/>
+        <v>4.7430350939300298E-9</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="11" spans="1:10">
+      <c r="B11">
         <v>3.92418975848453</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C11" s="12">
         <v>7.0694981791487397E-10</v>
       </c>
+      <c r="H11">
+        <v>5.7002656958327602</v>
+      </c>
+      <c r="I11">
+        <v>9.5768052809248296E-6</v>
+      </c>
+      <c r="J11" s="12">
+        <f t="shared" si="0"/>
+        <v>9.5768052809248291E-9</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11">
+    <row r="12" spans="1:10">
+      <c r="B12">
         <v>4.26053645543091</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C12" s="12">
         <v>1.2103279978808101E-9</v>
       </c>
+      <c r="H12">
+        <v>7.7281953503475203</v>
+      </c>
+      <c r="I12">
+        <v>1.7045584328470599E-5</v>
+      </c>
+      <c r="J12" s="12">
+        <f t="shared" si="0"/>
+        <v>1.7045584328470601E-8</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+    <row r="13" spans="1:10" ht="15">
+      <c r="A13" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B13" s="13">
         <v>4.9708261164373901</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C13" s="14">
         <v>1.8879755982172998E-9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="13">
-        <v>5.68151667583028</v>
-      </c>
-      <c r="C13" s="14">
-        <v>3.0855617283107602E-9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" s="15"/>
       <c r="B14" s="13">
-        <v>6.1054022965853303</v>
+        <v>5.68151667583028</v>
       </c>
       <c r="C14" s="14">
-        <v>4.7000388661768204E-9</v>
+        <v>3.0855617283107602E-9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" s="15"/>
       <c r="B15" s="13">
-        <v>6.4274057103154103</v>
+        <v>6.1054022965853303</v>
       </c>
       <c r="C15" s="14">
-        <v>5.8012158081172899E-9</v>
+        <v>4.7000388661768204E-9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="15"/>
       <c r="B16" s="13">
-        <v>7.0504085813783801</v>
+        <v>6.4274057103154103</v>
       </c>
       <c r="C16" s="14">
-        <v>6.2252616355228199E-9</v>
+        <v>5.8012158081172899E-9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" s="15"/>
       <c r="B17" s="13">
-        <v>7.3463468385524404</v>
+        <v>7.0504085813783801</v>
       </c>
       <c r="C17" s="14">
-        <v>9.2621531229420905E-9</v>
+        <v>6.2252616355228199E-9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15">
       <c r="A18" s="15"/>
       <c r="B18" s="13">
-        <v>8.0584218776148209</v>
+        <v>7.3463468385524404</v>
       </c>
       <c r="C18" s="14">
-        <v>1.1170566058489E-8</v>
+        <v>9.2621531229420905E-9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15">
       <c r="A19" s="15"/>
       <c r="B19" s="13">
-        <v>8.4834289824407207</v>
+        <v>8.0584218776148209</v>
       </c>
       <c r="C19" s="14">
-        <v>1.5138138132431501E-8</v>
+        <v>1.1170566058489E-8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15">
       <c r="A20" s="15"/>
       <c r="B20" s="13">
-        <v>8.8395177337443602</v>
+        <v>8.4834289824407207</v>
       </c>
       <c r="C20" s="14">
-        <v>2.05138464987828E-8</v>
+        <v>1.5138138132431501E-8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15">
       <c r="A21" s="15"/>
       <c r="B21" s="13">
-        <v>9.4018709487762901</v>
+        <v>8.8395177337443602</v>
       </c>
       <c r="C21" s="14">
-        <v>2.65324389685152E-8</v>
+        <v>2.05138464987828E-8</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15">
       <c r="A22" s="15"/>
       <c r="B22" s="13">
-        <v>10.3131861603009</v>
+        <v>9.4018709487762901</v>
       </c>
       <c r="C22" s="14">
-        <v>3.5963755482158002E-8</v>
+        <v>2.65324389685152E-8</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15">
       <c r="A23" s="15"/>
       <c r="B23" s="13">
-        <v>11.5478198468945</v>
+        <v>10.3131861603009</v>
       </c>
       <c r="C23" s="14">
-        <v>5.4792715714254297E-8</v>
+        <v>3.5963755482158002E-8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15">
       <c r="A24" s="15"/>
       <c r="B24" s="13">
-        <v>13.063857322002301</v>
+        <v>11.5478198468945</v>
       </c>
       <c r="C24" s="14">
-        <v>8.7476845978345504E-8</v>
+        <v>5.4792715714254297E-8</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15">
       <c r="A25" s="15"/>
       <c r="B25" s="13">
-        <v>14.778925406905101</v>
+        <v>13.063857322002301</v>
       </c>
       <c r="C25" s="14">
-        <v>1.10564098817298E-7</v>
+        <v>8.7476845978345504E-8</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15">
       <c r="A26" s="15"/>
       <c r="B26" s="13">
-        <v>16.2114338519455</v>
+        <v>14.778925406905101</v>
       </c>
       <c r="C26" s="14">
-        <v>1.3972277746978999E-7</v>
+        <v>1.10564098817298E-7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15">
       <c r="A27" s="15"/>
       <c r="B27" s="13">
-        <v>17.24277427362</v>
+        <v>16.2114338519455</v>
       </c>
       <c r="C27" s="14">
-        <v>1.89359517224642E-7</v>
+        <v>1.3972277746978999E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15">
       <c r="A28" s="15"/>
       <c r="B28" s="13">
+        <v>17.24277427362</v>
+      </c>
+      <c r="C28" s="14">
+        <v>1.89359517224642E-7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15">
+      <c r="A29" s="15"/>
+      <c r="B29" s="13">
         <v>18.914101456267801</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C29" s="14">
         <v>2.4495434361906002E-7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29">
+    <row r="30" spans="1:3">
+      <c r="B30">
         <v>20.747428935801199</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C30" s="12">
         <v>2.8860472832206001E-7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30">
+    <row r="31" spans="1:3">
+      <c r="B31">
         <v>23.713737056616502</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C31" s="12">
         <v>3.3225183737901698E-7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31">
+    <row r="32" spans="1:3">
+      <c r="B32">
         <v>26.826957952797201</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C32" s="12">
         <v>4.5042572723190799E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32">
+    <row r="33" spans="2:3">
+      <c r="B33">
         <v>29.731326465101301</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C33" s="12">
         <v>6.8621203935267004E-7</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33">
+    <row r="34" spans="2:3">
+      <c r="B34">
         <v>32.950130794918003</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C34" s="12">
         <v>9.5216840843197095E-7</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34">
+    <row r="35" spans="2:3">
+      <c r="B35">
         <v>36.894725687781197</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>1.52006238786628E-6</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35">
+    <row r="36" spans="2:3">
+      <c r="B36">
         <v>40.057013926518202</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>2.4836251598394602E-6</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36">
+    <row r="37" spans="2:3">
+      <c r="B37">
         <v>43.939705607607898</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>3.78354192522973E-6</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37">
+    <row r="38" spans="2:3">
+      <c r="B38">
         <v>46.257118042797899</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>6.0382393784068498E-6</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38">
-        <v>48.696752516586301</v>
-      </c>
-      <c r="C38">
-        <v>9.8643171969822904E-6</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3">
       <c r="B39">
         <v>48.696752516586301</v>
       </c>
       <c r="C39">
+        <v>9.8643171969822904E-6</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40">
+        <v>48.696752516586301</v>
+      </c>
+      <c r="C40">
         <v>1.6881085220425599E-5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A12:A28"/>
+    <mergeCell ref="A13:A29"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27600,22 +28121,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035D9A79-C5C3-4B01-9107-64EA0BCBB23E}">
   <dimension ref="A1:T137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L72" sqref="L72"/>
+    <sheetView topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T7" sqref="A7:T17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="9.19921875" customWidth="1"/>
-    <col min="3" max="3" width="9.69921875" customWidth="1"/>
-    <col min="10" max="10" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.8984375" customWidth="1"/>
-    <col min="13" max="13" width="9.69921875" customWidth="1"/>
-    <col min="16" max="16" width="9.69921875" customWidth="1"/>
+    <col min="2" max="2" width="9.25" customWidth="1"/>
+    <col min="3" max="3" width="9.75" customWidth="1"/>
+    <col min="10" max="10" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.875" customWidth="1"/>
+    <col min="13" max="13" width="9.75" customWidth="1"/>
+    <col min="16" max="16" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="A1" s="9" t="s">
         <v>39</v>
       </c>
@@ -27623,7 +28144,7 @@
         <v>6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="A2" s="9" t="s">
         <v>42</v>
       </c>
@@ -27631,7 +28152,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20">
       <c r="A3" s="9" t="s">
         <v>53</v>
       </c>
@@ -27640,7 +28161,7 @@
         <v>3.3672000000000003E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20">
       <c r="A4" s="9" t="s">
         <v>45</v>
       </c>
@@ -27648,11 +28169,11 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="B6" t="s">
         <v>28</v>
       </c>
@@ -27660,7 +28181,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -27707,7 +28228,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="A8" s="4">
         <v>0</v>
       </c>
@@ -27726,7 +28247,7 @@
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20">
       <c r="A9" s="4">
         <v>20000</v>
       </c>
@@ -27745,7 +28266,7 @@
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" s="4">
         <v>50000</v>
       </c>
@@ -27764,7 +28285,7 @@
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20">
       <c r="A11" s="4">
         <v>80000</v>
       </c>
@@ -27821,7 +28342,7 @@
         <v>2.4657239891062601</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20">
       <c r="A12" s="4">
         <v>90000</v>
       </c>
@@ -27878,7 +28399,7 @@
         <v>2.6863781352555374</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20">
       <c r="A13" s="4">
         <v>91000</v>
       </c>
@@ -27935,7 +28456,7 @@
         <v>2.7081900654716731</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20">
       <c r="A14" s="4">
         <v>92000</v>
       </c>
@@ -27992,7 +28513,7 @@
         <v>2.7299541401857046</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20">
       <c r="A15" s="4">
         <v>95000</v>
       </c>
@@ -28049,7 +28570,7 @@
         <v>2.7950062437645897</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="A16" s="4">
         <v>100000</v>
       </c>
@@ -28106,7 +28627,7 @@
         <v>2.9026270035976887</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="A17" s="4">
         <v>105000</v>
       </c>
@@ -28163,12 +28684,12 @@
         <v>3.0093121888074754</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20">
       <c r="B18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -28215,7 +28736,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20">
       <c r="A20" s="4">
         <v>0</v>
       </c>
@@ -28234,7 +28755,7 @@
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20">
       <c r="A21" s="4">
         <v>20000</v>
       </c>
@@ -28253,7 +28774,7 @@
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20">
       <c r="A22" s="4">
         <v>50000</v>
       </c>
@@ -28272,7 +28793,7 @@
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20">
       <c r="A23" s="4">
         <v>80000</v>
       </c>
@@ -28329,7 +28850,7 @@
         <v>2.2738431839905862</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20">
       <c r="A24" s="4">
         <v>90000</v>
       </c>
@@ -28386,7 +28907,7 @@
         <v>2.7732156829370309</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20">
       <c r="A25" s="4">
         <v>91000</v>
       </c>
@@ -28443,7 +28964,7 @@
         <v>2.8245635293742746</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20">
       <c r="A26" s="4">
         <v>92000</v>
       </c>
@@ -28500,7 +29021,7 @@
         <v>2.8761071319230873</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20">
       <c r="A27" s="4">
         <v>95000</v>
       </c>
@@ -28557,7 +29078,7 @@
         <v>3.0316538236102546</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20">
       <c r="A28" s="4">
         <v>100000</v>
       </c>
@@ -28614,7 +29135,7 @@
         <v>3.2929648158035167</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20">
       <c r="A29" s="4">
         <v>105000</v>
       </c>
@@ -28671,12 +29192,12 @@
         <v>3.5550022679102113</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20">
       <c r="B30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -28723,7 +29244,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20">
       <c r="A32" s="4">
         <v>0</v>
       </c>
@@ -28742,7 +29263,7 @@
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20">
       <c r="A33" s="4">
         <v>20000</v>
       </c>
@@ -28761,7 +29282,7 @@
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20">
       <c r="A34" s="4">
         <v>50000</v>
       </c>
@@ -28780,7 +29301,7 @@
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20">
       <c r="A35" s="4">
         <v>80000</v>
       </c>
@@ -28799,7 +29320,7 @@
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20">
       <c r="A36" s="4">
         <v>90000</v>
       </c>
@@ -28818,7 +29339,7 @@
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20">
       <c r="A37" s="4">
         <v>91000</v>
       </c>
@@ -28837,7 +29358,7 @@
       <c r="S37" s="5"/>
       <c r="T37" s="5"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20">
       <c r="A38" s="4">
         <v>92000</v>
       </c>
@@ -28856,7 +29377,7 @@
       <c r="S38" s="5"/>
       <c r="T38" s="5"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20">
       <c r="A39" s="4">
         <v>95000</v>
       </c>
@@ -28875,7 +29396,7 @@
       <c r="S39" s="5"/>
       <c r="T39" s="5"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20">
       <c r="A40" s="4">
         <v>100000</v>
       </c>
@@ -28932,7 +29453,7 @@
         <v>2.1567149736624489</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20">
       <c r="A41" s="4">
         <v>105000</v>
       </c>
@@ -28989,12 +29510,12 @@
         <v>2.6669976369331874</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20">
       <c r="B42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -29041,7 +29562,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20">
       <c r="A44" s="4">
         <v>0</v>
       </c>
@@ -29060,7 +29581,7 @@
       <c r="S44" s="5"/>
       <c r="T44" s="5"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20">
       <c r="A45" s="4">
         <v>20000</v>
       </c>
@@ -29079,7 +29600,7 @@
       <c r="S45" s="5"/>
       <c r="T45" s="5"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20">
       <c r="A46" s="4">
         <v>50000</v>
       </c>
@@ -29098,7 +29619,7 @@
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20">
       <c r="A47" s="4">
         <v>80000</v>
       </c>
@@ -29117,7 +29638,7 @@
       <c r="S47" s="5"/>
       <c r="T47" s="5"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20">
       <c r="A48" s="4">
         <v>90000</v>
       </c>
@@ -29136,7 +29657,7 @@
       <c r="S48" s="5"/>
       <c r="T48" s="5"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20">
       <c r="A49" s="4">
         <v>91000</v>
       </c>
@@ -29155,7 +29676,7 @@
       <c r="S49" s="5"/>
       <c r="T49" s="5"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20">
       <c r="A50" s="4">
         <v>92000</v>
       </c>
@@ -29174,7 +29695,7 @@
       <c r="S50" s="5"/>
       <c r="T50" s="5"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20">
       <c r="A51" s="4">
         <v>95000</v>
       </c>
@@ -29231,7 +29752,7 @@
         <v>1.3223621499411768</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20">
       <c r="A52" s="4">
         <v>100000</v>
       </c>
@@ -29288,7 +29809,7 @@
         <v>1.5996749193159243</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20">
       <c r="A53" s="4">
         <v>105000</v>
       </c>
@@ -29345,12 +29866,12 @@
         <v>1.9189635478254445</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20">
       <c r="B54" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -29397,7 +29918,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20">
       <c r="A56" s="4">
         <v>0</v>
       </c>
@@ -29416,7 +29937,7 @@
       <c r="S56" s="5"/>
       <c r="T56" s="5"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20">
       <c r="A57" s="4">
         <v>20000</v>
       </c>
@@ -29435,7 +29956,7 @@
       <c r="S57" s="5"/>
       <c r="T57" s="5"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20">
       <c r="A58" s="4">
         <v>50000</v>
       </c>
@@ -29454,7 +29975,7 @@
       <c r="S58" s="5"/>
       <c r="T58" s="5"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20">
       <c r="A59" s="4">
         <v>80000</v>
       </c>
@@ -29511,7 +30032,7 @@
         <v>3.1562457749298654</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20">
       <c r="A60" s="4">
         <v>90000</v>
       </c>
@@ -29568,7 +30089,7 @@
         <v>5.0107411294494142</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20">
       <c r="A61" s="4">
         <v>91000</v>
       </c>
@@ -29625,7 +30146,7 @@
         <v>5.236947881831707</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20">
       <c r="A62" s="4">
         <v>92000</v>
       </c>
@@ -29682,7 +30203,7 @@
         <v>5.472113151444419</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20">
       <c r="A63" s="4">
         <v>95000</v>
       </c>
@@ -29739,7 +30260,7 @@
         <v>6.2384189779610564</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20">
       <c r="A64" s="4">
         <v>100000</v>
       </c>
@@ -29796,7 +30317,7 @@
         <v>7.7804041845016236</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20">
       <c r="A65" s="4">
         <v>105000</v>
       </c>
@@ -29853,12 +30374,12 @@
         <v>9.8360645257767434</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20">
       <c r="B66" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -29905,7 +30426,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20">
       <c r="A68" s="4">
         <v>0</v>
       </c>
@@ -29924,7 +30445,7 @@
       <c r="S68" s="5"/>
       <c r="T68" s="5"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20">
       <c r="A69" s="4">
         <v>20000</v>
       </c>
@@ -29943,7 +30464,7 @@
       <c r="S69" s="5"/>
       <c r="T69" s="5"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20">
       <c r="A70" s="4">
         <v>50000</v>
       </c>
@@ -29962,7 +30483,7 @@
       <c r="S70" s="5"/>
       <c r="T70" s="5"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20">
       <c r="A71" s="4">
         <v>80000</v>
       </c>
@@ -30019,7 +30540,7 @@
         <v>2.2035083087399476</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20">
       <c r="A72" s="4">
         <v>90000</v>
       </c>
@@ -30076,7 +30597,7 @@
         <v>2.9467095783203803</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20">
       <c r="A73" s="4">
         <v>91000</v>
       </c>
@@ -30133,7 +30654,7 @@
         <v>3.0313128410931189</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20">
       <c r="A74" s="4">
         <v>92000</v>
       </c>
@@ -30190,7 +30711,7 @@
         <v>3.1179273242719994</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20">
       <c r="A75" s="4">
         <v>95000</v>
       </c>
@@ -30247,7 +30768,7 @@
         <v>3.390177135273166</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20">
       <c r="A76" s="4">
         <v>100000</v>
       </c>
@@ -30304,7 +30825,7 @@
         <v>3.8879465632624899</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20">
       <c r="A77" s="4">
         <v>105000</v>
       </c>
@@ -30361,12 +30882,12 @@
         <v>4.4472281367591817</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20">
       <c r="B78" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
@@ -30413,7 +30934,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20">
       <c r="A80" s="4">
         <v>0</v>
       </c>
@@ -30432,7 +30953,7 @@
       <c r="S80" s="5"/>
       <c r="T80" s="5"/>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20">
       <c r="A81" s="4">
         <v>20000</v>
       </c>
@@ -30451,7 +30972,7 @@
       <c r="S81" s="5"/>
       <c r="T81" s="5"/>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20">
       <c r="A82" s="4">
         <v>50000</v>
       </c>
@@ -30470,7 +30991,7 @@
       <c r="S82" s="5"/>
       <c r="T82" s="5"/>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20">
       <c r="A83" s="4">
         <v>80000</v>
       </c>
@@ -30489,7 +31010,7 @@
       <c r="S83" s="5"/>
       <c r="T83" s="5"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20">
       <c r="A84" s="4">
         <v>90000</v>
       </c>
@@ -30508,7 +31029,7 @@
       <c r="S84" s="5"/>
       <c r="T84" s="5"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20">
       <c r="A85" s="4">
         <v>91000</v>
       </c>
@@ -30527,7 +31048,7 @@
       <c r="S85" s="5"/>
       <c r="T85" s="5"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20">
       <c r="A86" s="4">
         <v>92000</v>
       </c>
@@ -30546,7 +31067,7 @@
       <c r="S86" s="5"/>
       <c r="T86" s="5"/>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20">
       <c r="A87" s="4">
         <v>95000</v>
       </c>
@@ -30603,7 +31124,7 @@
         <v>2.3102856065648045</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20">
       <c r="A88" s="4">
         <v>100000</v>
       </c>
@@ -30660,7 +31181,7 @@
         <v>2.7504552573241101</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20">
       <c r="A89" s="4">
         <v>105000</v>
       </c>
@@ -30717,12 +31238,12 @@
         <v>3.2848400285157062</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20">
       <c r="B90" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20">
       <c r="A91" s="1" t="s">
         <v>0</v>
       </c>
@@ -30769,7 +31290,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20">
       <c r="A92" s="4">
         <v>0</v>
       </c>
@@ -30788,7 +31309,7 @@
       <c r="S92" s="5"/>
       <c r="T92" s="5"/>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20">
       <c r="A93" s="4">
         <v>20000</v>
       </c>
@@ -30807,7 +31328,7 @@
       <c r="S93" s="5"/>
       <c r="T93" s="5"/>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20">
       <c r="A94" s="4">
         <v>50000</v>
       </c>
@@ -30826,7 +31347,7 @@
       <c r="S94" s="5"/>
       <c r="T94" s="5"/>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20">
       <c r="A95" s="4">
         <v>80000</v>
       </c>
@@ -30845,7 +31366,7 @@
       <c r="S95" s="5"/>
       <c r="T95" s="5"/>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20">
       <c r="A96" s="4">
         <v>90000</v>
       </c>
@@ -30902,7 +31423,7 @@
         <v>2.0059266978222561</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20">
       <c r="A97" s="4">
         <v>91000</v>
       </c>
@@ -30959,7 +31480,7 @@
         <v>2.0762623691670248</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20">
       <c r="A98" s="4">
         <v>92000</v>
       </c>
@@ -31016,7 +31537,7 @@
         <v>2.1476964835930348</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20">
       <c r="A99" s="4">
         <v>95000</v>
       </c>
@@ -31073,7 +31594,7 @@
         <v>2.3670197750788846</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20">
       <c r="A100" s="4">
         <v>100000</v>
       </c>
@@ -31130,7 +31651,7 @@
         <v>2.7379071671330246</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20">
       <c r="A101" s="4">
         <v>105000</v>
       </c>
@@ -31187,12 +31708,12 @@
         <v>3.0882829446350515</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20">
       <c r="B102" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20">
       <c r="A103" s="1" t="s">
         <v>0</v>
       </c>
@@ -31239,7 +31760,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20">
       <c r="A104" s="4">
         <v>0</v>
       </c>
@@ -31258,7 +31779,7 @@
       <c r="S104" s="5"/>
       <c r="T104" s="5"/>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20">
       <c r="A105" s="4">
         <v>20000</v>
       </c>
@@ -31277,7 +31798,7 @@
       <c r="S105" s="5"/>
       <c r="T105" s="5"/>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20">
       <c r="A106" s="4">
         <v>50000</v>
       </c>
@@ -31296,7 +31817,7 @@
       <c r="S106" s="5"/>
       <c r="T106" s="5"/>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20">
       <c r="A107" s="4">
         <v>80000</v>
       </c>
@@ -31353,7 +31874,7 @@
         <v>2.2671002432128233</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20">
       <c r="A108" s="4">
         <v>90000</v>
       </c>
@@ -31410,7 +31931,7 @@
         <v>2.7157501285073753</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20">
       <c r="A109" s="4">
         <v>91000</v>
       </c>
@@ -31467,7 +31988,7 @@
         <v>2.7616643786869757</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20">
       <c r="A110" s="4">
         <v>92000</v>
       </c>
@@ -31524,7 +32045,7 @@
         <v>2.8077493216551379</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20">
       <c r="A111" s="4">
         <v>95000</v>
       </c>
@@ -31581,7 +32102,7 @@
         <v>2.9470203813577358</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20">
       <c r="A112" s="4">
         <v>100000</v>
       </c>
@@ -31638,7 +32159,7 @@
         <v>3.1824093966890858</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20">
       <c r="A113" s="4">
         <v>105000</v>
       </c>
@@ -31695,12 +32216,12 @@
         <v>3.421844114598442</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20">
       <c r="B114" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20">
       <c r="A115" s="1" t="s">
         <v>0</v>
       </c>
@@ -31747,7 +32268,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20">
       <c r="A116" s="4">
         <v>0</v>
       </c>
@@ -31766,7 +32287,7 @@
       <c r="S116" s="5"/>
       <c r="T116" s="5"/>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20">
       <c r="A117" s="4">
         <v>20000</v>
       </c>
@@ -31785,7 +32306,7 @@
       <c r="S117" s="5"/>
       <c r="T117" s="5"/>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20">
       <c r="A118" s="4">
         <v>50000</v>
       </c>
@@ -31804,7 +32325,7 @@
       <c r="S118" s="5"/>
       <c r="T118" s="5"/>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20">
       <c r="A119" s="4">
         <v>80000</v>
       </c>
@@ -31823,7 +32344,7 @@
       <c r="S119" s="5"/>
       <c r="T119" s="5"/>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20">
       <c r="A120" s="4">
         <v>90000</v>
       </c>
@@ -31880,7 +32401,7 @@
         <v>2.749188735959152</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20">
       <c r="A121" s="4">
         <v>91000</v>
       </c>
@@ -31937,7 +32458,7 @@
         <v>2.7961745842832388</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20">
       <c r="A122" s="4">
         <v>92000</v>
       </c>
@@ -31994,7 +32515,7 @@
         <v>2.8432554676872845</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20">
       <c r="A123" s="4">
         <v>95000</v>
       </c>
@@ -32051,7 +32572,7 @@
         <v>2.985076108336346</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20">
       <c r="A124" s="4">
         <v>100000</v>
       </c>
@@ -32108,7 +32629,7 @@
         <v>3.2230329157979258</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20">
       <c r="A125" s="4">
         <v>105000</v>
       </c>
@@ -32165,12 +32686,12 @@
         <v>3.4626783132164296</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20">
       <c r="B126" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20">
       <c r="A127" s="1" t="s">
         <v>0</v>
       </c>
@@ -32217,7 +32738,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20">
       <c r="A128" s="4">
         <v>0</v>
       </c>
@@ -32236,7 +32757,7 @@
       <c r="S128" s="5"/>
       <c r="T128" s="5"/>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20">
       <c r="A129" s="4">
         <v>20000</v>
       </c>
@@ -32255,7 +32776,7 @@
       <c r="S129" s="5"/>
       <c r="T129" s="5"/>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20">
       <c r="A130" s="4">
         <v>50000</v>
       </c>
@@ -32274,7 +32795,7 @@
       <c r="S130" s="5"/>
       <c r="T130" s="5"/>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20">
       <c r="A131" s="4">
         <v>80000</v>
       </c>
@@ -32331,7 +32852,7 @@
         <v>2.8026867826644564</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20">
       <c r="A132" s="4">
         <v>90000</v>
       </c>
@@ -32388,7 +32909,7 @@
         <v>3.4123586724492876</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20">
       <c r="A133" s="4">
         <v>91000</v>
       </c>
@@ -32445,7 +32966,7 @@
         <v>3.4756090814858887</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20">
       <c r="A134" s="4">
         <v>92000</v>
       </c>
@@ -32502,7 +33023,7 @@
         <v>3.5392983475823421</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:20">
       <c r="A135" s="4">
         <v>95000</v>
       </c>
@@ -32559,7 +33080,7 @@
         <v>3.7331238893426004</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20">
       <c r="A136" s="4">
         <v>100000</v>
       </c>
@@ -32616,7 +33137,7 @@
         <v>4.0661240328453552</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20">
       <c r="A137" s="4">
         <v>105000</v>
       </c>
@@ -32689,22 +33210,22 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="10.69921875" customWidth="1"/>
-    <col min="3" max="3" width="9.19921875" customWidth="1"/>
-    <col min="4" max="4" width="8.19921875" customWidth="1"/>
+    <col min="1" max="2" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="9.25" customWidth="1"/>
+    <col min="4" max="4" width="8.25" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="9.69921875" customWidth="1"/>
-    <col min="7" max="7" width="10.69921875" customWidth="1"/>
-    <col min="8" max="8" width="13.59765625" customWidth="1"/>
-    <col min="9" max="10" width="10.19921875" customWidth="1"/>
-    <col min="11" max="11" width="10.59765625" customWidth="1"/>
-    <col min="12" max="12" width="11.69921875" customWidth="1"/>
-    <col min="13" max="13" width="10.19921875" customWidth="1"/>
-    <col min="14" max="14" width="11.3984375" customWidth="1"/>
+    <col min="6" max="6" width="9.75" customWidth="1"/>
+    <col min="7" max="7" width="10.75" customWidth="1"/>
+    <col min="8" max="8" width="13.625" customWidth="1"/>
+    <col min="9" max="10" width="10.25" customWidth="1"/>
+    <col min="11" max="11" width="10.625" customWidth="1"/>
+    <col min="12" max="12" width="11.75" customWidth="1"/>
+    <col min="13" max="13" width="10.25" customWidth="1"/>
+    <col min="14" max="14" width="11.375" customWidth="1"/>
     <col min="15" max="15" width="9.5" customWidth="1"/>
-    <col min="16" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="16" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -32724,11 +33245,11 @@
       <selection sqref="A1:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="16" width="10.69921875" customWidth="1"/>
-    <col min="17" max="17" width="12.19921875" customWidth="1"/>
-    <col min="18" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="1" max="16" width="10.75" customWidth="1"/>
+    <col min="17" max="17" width="12.25" customWidth="1"/>
+    <col min="18" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -32748,13 +33269,13 @@
       <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="26" width="10.69921875" customWidth="1"/>
-    <col min="32" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="1" max="26" width="10.75" customWidth="1"/>
+    <col min="32" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -32816,7 +33337,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="A3">
         <v>80000</v>
       </c>
@@ -32842,7 +33363,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24">
       <c r="A4">
         <v>90000</v>
       </c>
@@ -32868,7 +33389,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="A5">
         <v>100000</v>
       </c>
@@ -32894,7 +33415,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24">
       <c r="A6">
         <v>105000</v>
       </c>
@@ -32920,7 +33441,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="A7">
         <v>115000</v>
       </c>
@@ -32946,7 +33467,7 @@
         <v>115000</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="A8">
         <v>125000</v>
       </c>
@@ -32972,7 +33493,7 @@
         <v>125000</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24">
       <c r="A9">
         <v>135000</v>
       </c>
@@ -33007,7 +33528,7 @@
         <v>135000</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24">
       <c r="A10">
         <v>145000</v>
       </c>
@@ -33042,7 +33563,7 @@
         <v>145000</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24">
       <c r="A11">
         <v>155000</v>
       </c>
@@ -33086,7 +33607,7 @@
         <v>3.92469713729365E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24">
       <c r="A12">
         <v>175000</v>
       </c>
@@ -33139,7 +33660,7 @@
         <v>5.0838484916259502E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="A13">
         <v>195000</v>
       </c>
@@ -33192,7 +33713,7 @@
         <v>0.12621611691672899</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24">
       <c r="A14">
         <v>215000</v>
       </c>
@@ -33254,7 +33775,7 @@
         <v>5.14299852570844E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24">
       <c r="A15">
         <v>225000</v>
       </c>
@@ -33316,7 +33837,7 @@
         <v>0.11391790821570499</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24">
       <c r="A16">
         <v>235000</v>
       </c>
@@ -33378,7 +33899,7 @@
         <v>6.5728018841552396E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24">
       <c r="A17">
         <v>245000</v>
       </c>
@@ -33440,7 +33961,7 @@
         <v>6.4449969207186694E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -33490,7 +34011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24">
       <c r="A22">
         <v>80000</v>
       </c>
@@ -33504,7 +34025,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24">
       <c r="A23">
         <v>90000</v>
       </c>
@@ -33518,7 +34039,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24">
       <c r="A24">
         <v>100000</v>
       </c>
@@ -33532,7 +34053,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24">
       <c r="A25">
         <v>105000</v>
       </c>
@@ -33546,7 +34067,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24">
       <c r="A26">
         <v>115000</v>
       </c>
@@ -33560,7 +34081,7 @@
         <v>115000</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24">
       <c r="A27">
         <v>125000</v>
       </c>
@@ -33574,7 +34095,7 @@
         <v>125000</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24">
       <c r="A28">
         <v>135000</v>
       </c>
@@ -33606,7 +34127,7 @@
         <v>0.28842538296747899</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24">
       <c r="A29">
         <v>145000</v>
       </c>
@@ -33638,7 +34159,7 @@
         <v>0.24612916781514799</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24">
       <c r="A30">
         <v>155000</v>
       </c>
@@ -33670,7 +34191,7 @@
         <v>0.41710503614362299</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24">
       <c r="A31">
         <v>175000</v>
       </c>
@@ -33711,7 +34232,7 @@
         <v>0.48465204324982197</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24">
       <c r="A32">
         <v>195000</v>
       </c>
@@ -33761,7 +34282,7 @@
         <v>0.550969778547587</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19">
       <c r="A33">
         <v>215000</v>
       </c>
@@ -33811,7 +34332,7 @@
         <v>1.0405666476426001</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19">
       <c r="A34">
         <v>225000</v>
       </c>
@@ -33861,7 +34382,7 @@
         <v>1.3650029220936299</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19">
       <c r="A35">
         <v>235000</v>
       </c>
@@ -33911,7 +34432,7 @@
         <v>1.5028270584451799</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19">
       <c r="A36">
         <v>245000</v>
       </c>
@@ -33977,18 +34498,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:J19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="6" width="10.69921875" customWidth="1"/>
-    <col min="7" max="7" width="10.3984375" customWidth="1"/>
-    <col min="8" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="1" max="6" width="10.75" customWidth="1"/>
+    <col min="7" max="7" width="10.375" customWidth="1"/>
+    <col min="8" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="A1" s="9" t="s">
         <v>39</v>
       </c>
@@ -33996,7 +34517,7 @@
         <v>6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="A2" s="9" t="s">
         <v>42</v>
       </c>
@@ -34004,7 +34525,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20">
       <c r="A3" s="9" t="s">
         <v>53</v>
       </c>
@@ -34013,7 +34534,7 @@
         <v>3.3611000000000005E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20">
       <c r="A4" s="9" t="s">
         <v>45</v>
       </c>
@@ -34021,11 +34542,11 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="B6" t="s">
         <v>28</v>
       </c>
@@ -34033,7 +34554,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -34080,7 +34601,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="A8" s="4">
         <v>0</v>
       </c>
@@ -34099,7 +34620,7 @@
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20">
       <c r="A9" s="4">
         <v>80000</v>
       </c>
@@ -34156,7 +34677,7 @@
         <v>2.5691156368612411</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" s="4">
         <v>90000</v>
       </c>
@@ -34213,7 +34734,7 @@
         <v>2.8548863254273846</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20">
       <c r="A11" s="4">
         <v>100000</v>
       </c>
@@ -34270,7 +34791,7 @@
         <v>3.2290630084439358</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20">
       <c r="A12" s="4">
         <v>105000</v>
       </c>
@@ -34327,7 +34848,7 @@
         <v>3.4573351136996981</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20">
       <c r="A13" s="4">
         <v>115000</v>
       </c>
@@ -34384,7 +34905,7 @@
         <v>4.0151752182393903</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20">
       <c r="A14" s="4">
         <v>125000</v>
       </c>
@@ -34441,7 +34962,7 @@
         <v>4.7408819917995695</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20">
       <c r="A15" s="6">
         <v>130000</v>
       </c>
@@ -34498,7 +35019,7 @@
         <v>5.1845518513000108</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="A16" s="8">
         <v>135000</v>
       </c>
@@ -34555,7 +35076,7 @@
         <v>5.6978702140259516</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="A17" s="4">
         <v>140000</v>
       </c>
@@ -34612,7 +35133,7 @@
         <v>6.3004931800512765</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20">
       <c r="A18" s="4">
         <v>150000</v>
       </c>
@@ -34669,7 +35190,7 @@
         <v>7.9148864561189258</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20">
       <c r="A19" s="4">
         <v>160000</v>
       </c>

</xml_diff>

<commit_message>
measured the size of AMYa part
</commit_message>
<xml_diff>
--- a/crack_size_growth_v2.xlsx
+++ b/crack_size_growth_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Research\AM_fatigue\fatigue-crack-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F46F95-446F-4CC6-B3CE-7E67CC8B8498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6404DE0-4D69-462D-95C7-A7280E548687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="3000" windowWidth="10620" windowHeight="9795" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="165" yWindow="1275" windowWidth="11115" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ref_dadN-dK" sheetId="6" r:id="rId1"/>
@@ -26862,8 +26862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="E191" sqref="E191"/>
+    <sheetView topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="F232" sqref="F232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -27940,71 +27940,111 @@
       <c r="A113" s="4">
         <v>90000</v>
       </c>
-      <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
+      <c r="B113" s="5">
+        <v>29</v>
+      </c>
+      <c r="C113" s="5">
+        <v>45</v>
+      </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="4">
         <v>95000</v>
       </c>
-      <c r="B114" s="5"/>
-      <c r="C114" s="5"/>
+      <c r="B114" s="5">
+        <v>30</v>
+      </c>
+      <c r="C114" s="5">
+        <v>46</v>
+      </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="4">
         <v>100000</v>
       </c>
-      <c r="B115" s="5"/>
-      <c r="C115" s="5"/>
+      <c r="B115" s="5">
+        <v>35</v>
+      </c>
+      <c r="C115" s="5">
+        <v>53</v>
+      </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="4">
         <v>105000</v>
       </c>
-      <c r="B116" s="5"/>
-      <c r="C116" s="5"/>
+      <c r="B116" s="5">
+        <v>39</v>
+      </c>
+      <c r="C116" s="5">
+        <v>56</v>
+      </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="4">
         <v>110000</v>
       </c>
-      <c r="B117" s="5"/>
-      <c r="C117" s="5"/>
+      <c r="B117" s="5">
+        <v>42</v>
+      </c>
+      <c r="C117" s="5">
+        <v>56</v>
+      </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="6">
         <v>115000</v>
       </c>
-      <c r="B118" s="7"/>
-      <c r="C118" s="7"/>
+      <c r="B118" s="7">
+        <v>43</v>
+      </c>
+      <c r="C118" s="7">
+        <v>64</v>
+      </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="8">
         <v>120000</v>
       </c>
-      <c r="B119" s="5"/>
-      <c r="C119" s="5"/>
+      <c r="B119" s="5">
+        <v>46</v>
+      </c>
+      <c r="C119" s="5">
+        <v>66</v>
+      </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="4">
         <v>125000</v>
       </c>
-      <c r="B120" s="5"/>
-      <c r="C120" s="5"/>
+      <c r="B120" s="5">
+        <v>47</v>
+      </c>
+      <c r="C120" s="5">
+        <v>75</v>
+      </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="4">
         <v>130000</v>
       </c>
-      <c r="B121" s="5"/>
-      <c r="C121" s="5"/>
+      <c r="B121" s="5">
+        <v>52</v>
+      </c>
+      <c r="C121" s="5">
+        <v>92</v>
+      </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="4">
         <v>140000</v>
       </c>
-      <c r="B122" s="5"/>
-      <c r="C122" s="5"/>
+      <c r="B122" s="5">
+        <v>62</v>
+      </c>
+      <c r="C122" s="5">
+        <v>118</v>
+      </c>
     </row>
     <row r="123" spans="1:3">
       <c r="B123" t="s">
@@ -28082,22 +28122,34 @@
       <c r="A133" s="4">
         <v>125000</v>
       </c>
-      <c r="B133" s="5"/>
-      <c r="C133" s="5"/>
+      <c r="B133" s="5">
+        <v>18</v>
+      </c>
+      <c r="C133" s="5">
+        <v>32</v>
+      </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="4">
         <v>130000</v>
       </c>
-      <c r="B134" s="5"/>
-      <c r="C134" s="5"/>
+      <c r="B134" s="5">
+        <v>22</v>
+      </c>
+      <c r="C134" s="5">
+        <v>36</v>
+      </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="4">
         <v>140000</v>
       </c>
-      <c r="B135" s="5"/>
-      <c r="C135" s="5"/>
+      <c r="B135" s="5">
+        <v>40</v>
+      </c>
+      <c r="C135" s="5">
+        <v>51</v>
+      </c>
     </row>
     <row r="136" spans="1:3">
       <c r="B136" t="s">
@@ -28119,78 +28171,122 @@
       <c r="A138" s="4">
         <v>80000</v>
       </c>
-      <c r="B138" s="5"/>
-      <c r="C138" s="5"/>
+      <c r="B138" s="5">
+        <v>44</v>
+      </c>
+      <c r="C138" s="5">
+        <v>88</v>
+      </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="4">
         <v>90000</v>
       </c>
-      <c r="B139" s="5"/>
-      <c r="C139" s="5"/>
+      <c r="B139" s="5">
+        <v>58</v>
+      </c>
+      <c r="C139" s="5">
+        <v>122</v>
+      </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="4">
         <v>95000</v>
       </c>
-      <c r="B140" s="5"/>
-      <c r="C140" s="5"/>
+      <c r="B140" s="5">
+        <v>61</v>
+      </c>
+      <c r="C140" s="5">
+        <v>131</v>
+      </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="4">
         <v>100000</v>
       </c>
-      <c r="B141" s="5"/>
-      <c r="C141" s="5"/>
+      <c r="B141" s="5">
+        <v>62</v>
+      </c>
+      <c r="C141" s="5">
+        <v>136</v>
+      </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="4">
         <v>105000</v>
       </c>
-      <c r="B142" s="5"/>
-      <c r="C142" s="5"/>
+      <c r="B142" s="5">
+        <v>67</v>
+      </c>
+      <c r="C142" s="5">
+        <v>146</v>
+      </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="4">
         <v>110000</v>
       </c>
-      <c r="B143" s="5"/>
-      <c r="C143" s="5"/>
+      <c r="B143" s="5">
+        <v>70</v>
+      </c>
+      <c r="C143" s="5">
+        <v>170</v>
+      </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="6">
         <v>115000</v>
       </c>
-      <c r="B144" s="7"/>
-      <c r="C144" s="7"/>
+      <c r="B144" s="7">
+        <v>78</v>
+      </c>
+      <c r="C144" s="7">
+        <v>188</v>
+      </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="8">
         <v>120000</v>
       </c>
-      <c r="B145" s="5"/>
-      <c r="C145" s="5"/>
+      <c r="B145" s="5">
+        <v>84</v>
+      </c>
+      <c r="C145" s="5">
+        <v>218</v>
+      </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="4">
         <v>125000</v>
       </c>
-      <c r="B146" s="5"/>
-      <c r="C146" s="5"/>
+      <c r="B146" s="5">
+        <v>94</v>
+      </c>
+      <c r="C146" s="5">
+        <v>232</v>
+      </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="4">
         <v>130000</v>
       </c>
-      <c r="B147" s="5"/>
-      <c r="C147" s="5"/>
+      <c r="B147" s="5">
+        <v>108</v>
+      </c>
+      <c r="C147" s="5">
+        <v>280</v>
+      </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="4">
         <v>140000</v>
       </c>
-      <c r="B148" s="5"/>
-      <c r="C148" s="5"/>
+      <c r="B148" s="5">
+        <v>138</v>
+      </c>
+      <c r="C148" s="5">
+        <v>430</v>
+      </c>
     </row>
     <row r="149" spans="1:3">
       <c r="B149" t="s">
@@ -28233,57 +28329,89 @@
       <c r="A154" s="4">
         <v>100000</v>
       </c>
-      <c r="B154" s="5"/>
-      <c r="C154" s="5"/>
+      <c r="B154" s="5">
+        <v>28</v>
+      </c>
+      <c r="C154" s="5">
+        <v>29</v>
+      </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="4">
         <v>105000</v>
       </c>
-      <c r="B155" s="5"/>
-      <c r="C155" s="5"/>
+      <c r="B155" s="5">
+        <v>30</v>
+      </c>
+      <c r="C155" s="5">
+        <v>33</v>
+      </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="4">
         <v>110000</v>
       </c>
-      <c r="B156" s="5"/>
-      <c r="C156" s="5"/>
+      <c r="B156" s="5">
+        <v>38</v>
+      </c>
+      <c r="C156" s="5">
+        <v>59</v>
+      </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="6">
         <v>115000</v>
       </c>
-      <c r="B157" s="7"/>
-      <c r="C157" s="7"/>
+      <c r="B157" s="7">
+        <v>45</v>
+      </c>
+      <c r="C157" s="7">
+        <v>67</v>
+      </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="8">
         <v>120000</v>
       </c>
-      <c r="B158" s="5"/>
-      <c r="C158" s="5"/>
+      <c r="B158" s="5">
+        <v>48</v>
+      </c>
+      <c r="C158" s="5">
+        <v>72</v>
+      </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="4">
         <v>125000</v>
       </c>
-      <c r="B159" s="5"/>
-      <c r="C159" s="5"/>
+      <c r="B159" s="5">
+        <v>53</v>
+      </c>
+      <c r="C159" s="5">
+        <v>78</v>
+      </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="4">
         <v>130000</v>
       </c>
-      <c r="B160" s="5"/>
-      <c r="C160" s="5"/>
+      <c r="B160" s="5">
+        <v>59</v>
+      </c>
+      <c r="C160" s="5">
+        <v>90</v>
+      </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="4">
         <v>140000</v>
       </c>
-      <c r="B161" s="5"/>
-      <c r="C161" s="5"/>
+      <c r="B161" s="5">
+        <v>70</v>
+      </c>
+      <c r="C161" s="5">
+        <v>108</v>
+      </c>
     </row>
     <row r="162" spans="1:3">
       <c r="B162" t="s">
@@ -28305,78 +28433,122 @@
       <c r="A164" s="4">
         <v>80000</v>
       </c>
-      <c r="B164" s="5"/>
-      <c r="C164" s="5"/>
+      <c r="B164" s="5">
+        <v>39</v>
+      </c>
+      <c r="C164" s="5">
+        <v>85</v>
+      </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="4">
         <v>90000</v>
       </c>
-      <c r="B165" s="5"/>
-      <c r="C165" s="5"/>
+      <c r="B165" s="5">
+        <v>43</v>
+      </c>
+      <c r="C165" s="5">
+        <v>86</v>
+      </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="4">
         <v>95000</v>
       </c>
-      <c r="B166" s="5"/>
-      <c r="C166" s="5"/>
+      <c r="B166" s="5">
+        <v>44</v>
+      </c>
+      <c r="C166" s="5">
+        <v>99</v>
+      </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="4">
         <v>100000</v>
       </c>
-      <c r="B167" s="5"/>
-      <c r="C167" s="5"/>
+      <c r="B167" s="5">
+        <v>51</v>
+      </c>
+      <c r="C167" s="5">
+        <v>108</v>
+      </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="4">
         <v>105000</v>
       </c>
-      <c r="B168" s="5"/>
-      <c r="C168" s="5"/>
+      <c r="B168" s="5">
+        <v>54</v>
+      </c>
+      <c r="C168" s="5">
+        <v>127</v>
+      </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="4">
         <v>110000</v>
       </c>
-      <c r="B169" s="5"/>
-      <c r="C169" s="5"/>
+      <c r="B169" s="5">
+        <v>66</v>
+      </c>
+      <c r="C169" s="5">
+        <v>138</v>
+      </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="6">
         <v>115000</v>
       </c>
-      <c r="B170" s="7"/>
-      <c r="C170" s="7"/>
+      <c r="B170" s="7">
+        <v>66</v>
+      </c>
+      <c r="C170" s="7">
+        <v>145</v>
+      </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="8">
         <v>120000</v>
       </c>
-      <c r="B171" s="5"/>
-      <c r="C171" s="5"/>
+      <c r="B171" s="5">
+        <v>68</v>
+      </c>
+      <c r="C171" s="5">
+        <v>155</v>
+      </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="4">
         <v>125000</v>
       </c>
-      <c r="B172" s="5"/>
-      <c r="C172" s="5"/>
+      <c r="B172" s="5">
+        <v>68</v>
+      </c>
+      <c r="C172" s="5">
+        <v>155</v>
+      </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="4">
         <v>130000</v>
       </c>
-      <c r="B173" s="5"/>
-      <c r="C173" s="5"/>
+      <c r="B173" s="5">
+        <v>76</v>
+      </c>
+      <c r="C173" s="5">
+        <v>184</v>
+      </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="4">
         <v>140000</v>
       </c>
-      <c r="B174" s="5"/>
-      <c r="C174" s="5"/>
+      <c r="B174" s="5">
+        <v>104</v>
+      </c>
+      <c r="C174" s="5">
+        <v>188</v>
+      </c>
     </row>
     <row r="175" spans="1:3">
       <c r="B175" t="s">
@@ -28398,78 +28570,122 @@
       <c r="A177" s="4">
         <v>80000</v>
       </c>
-      <c r="B177" s="5"/>
-      <c r="C177" s="5"/>
+      <c r="B177" s="5">
+        <v>37</v>
+      </c>
+      <c r="C177" s="5">
+        <v>83</v>
+      </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="4">
         <v>90000</v>
       </c>
-      <c r="B178" s="5"/>
-      <c r="C178" s="5"/>
+      <c r="B178" s="5">
+        <v>44</v>
+      </c>
+      <c r="C178" s="5">
+        <v>91</v>
+      </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="4">
         <v>95000</v>
       </c>
-      <c r="B179" s="5"/>
-      <c r="C179" s="5"/>
+      <c r="B179" s="5">
+        <v>48</v>
+      </c>
+      <c r="C179" s="5">
+        <v>98</v>
+      </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="4">
         <v>100000</v>
       </c>
-      <c r="B180" s="5"/>
-      <c r="C180" s="5"/>
+      <c r="B180" s="5">
+        <v>54</v>
+      </c>
+      <c r="C180" s="5">
+        <v>110</v>
+      </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="4">
         <v>105000</v>
       </c>
-      <c r="B181" s="5"/>
-      <c r="C181" s="5"/>
+      <c r="B181" s="5">
+        <v>56</v>
+      </c>
+      <c r="C181" s="5">
+        <v>119</v>
+      </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="4">
         <v>110000</v>
       </c>
-      <c r="B182" s="5"/>
-      <c r="C182" s="5"/>
+      <c r="B182" s="5">
+        <v>62</v>
+      </c>
+      <c r="C182" s="5">
+        <v>126</v>
+      </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="6">
         <v>115000</v>
       </c>
-      <c r="B183" s="7"/>
-      <c r="C183" s="7"/>
+      <c r="B183" s="7">
+        <v>62</v>
+      </c>
+      <c r="C183" s="7">
+        <v>132</v>
+      </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="8">
         <v>120000</v>
       </c>
-      <c r="B184" s="5"/>
-      <c r="C184" s="5"/>
+      <c r="B184" s="5">
+        <v>63</v>
+      </c>
+      <c r="C184" s="5">
+        <v>144</v>
+      </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="4">
         <v>125000</v>
       </c>
-      <c r="B185" s="5"/>
-      <c r="C185" s="5"/>
+      <c r="B185" s="5">
+        <v>76</v>
+      </c>
+      <c r="C185" s="5">
+        <v>159</v>
+      </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="4">
         <v>130000</v>
       </c>
-      <c r="B186" s="5"/>
-      <c r="C186" s="5"/>
+      <c r="B186" s="5">
+        <v>76</v>
+      </c>
+      <c r="C186" s="5">
+        <v>175</v>
+      </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="4">
         <v>140000</v>
       </c>
-      <c r="B187" s="5"/>
-      <c r="C187" s="5"/>
+      <c r="B187" s="5">
+        <v>85</v>
+      </c>
+      <c r="C187" s="5">
+        <v>257</v>
+      </c>
     </row>
     <row r="188" spans="1:3">
       <c r="B188" t="s">
@@ -28498,71 +28714,111 @@
       <c r="A191" s="4">
         <v>90000</v>
       </c>
-      <c r="B191" s="5"/>
-      <c r="C191" s="5"/>
+      <c r="B191" s="5">
+        <v>32</v>
+      </c>
+      <c r="C191" s="5">
+        <v>46</v>
+      </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="4">
         <v>95000</v>
       </c>
-      <c r="B192" s="5"/>
-      <c r="C192" s="5"/>
+      <c r="B192" s="5">
+        <v>36</v>
+      </c>
+      <c r="C192" s="5">
+        <v>48</v>
+      </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="4">
         <v>100000</v>
       </c>
-      <c r="B193" s="5"/>
-      <c r="C193" s="5"/>
+      <c r="B193" s="5">
+        <v>37</v>
+      </c>
+      <c r="C193" s="5">
+        <v>56</v>
+      </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="4">
         <v>105000</v>
       </c>
-      <c r="B194" s="5"/>
-      <c r="C194" s="5"/>
+      <c r="B194" s="5">
+        <v>42</v>
+      </c>
+      <c r="C194" s="5">
+        <v>59</v>
+      </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="4">
         <v>110000</v>
       </c>
-      <c r="B195" s="5"/>
-      <c r="C195" s="5"/>
+      <c r="B195" s="5">
+        <v>45</v>
+      </c>
+      <c r="C195" s="5">
+        <v>64</v>
+      </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="6">
         <v>115000</v>
       </c>
-      <c r="B196" s="7"/>
-      <c r="C196" s="7"/>
+      <c r="B196" s="7">
+        <v>49</v>
+      </c>
+      <c r="C196" s="7">
+        <v>67</v>
+      </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="8">
         <v>120000</v>
       </c>
-      <c r="B197" s="5"/>
-      <c r="C197" s="5"/>
+      <c r="B197" s="5">
+        <v>50</v>
+      </c>
+      <c r="C197" s="5">
+        <v>70</v>
+      </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="4">
         <v>125000</v>
       </c>
-      <c r="B198" s="5"/>
-      <c r="C198" s="5"/>
+      <c r="B198" s="5">
+        <v>51</v>
+      </c>
+      <c r="C198" s="5">
+        <v>73</v>
+      </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="4">
         <v>130000</v>
       </c>
-      <c r="B199" s="5"/>
-      <c r="C199" s="5"/>
+      <c r="B199" s="5">
+        <v>56</v>
+      </c>
+      <c r="C199" s="5">
+        <v>82</v>
+      </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="4">
         <v>140000</v>
       </c>
-      <c r="B200" s="5"/>
-      <c r="C200" s="5"/>
+      <c r="B200" s="5">
+        <v>61</v>
+      </c>
+      <c r="C200" s="5">
+        <v>97</v>
+      </c>
     </row>
     <row r="201" spans="1:3">
       <c r="B201" t="s">
@@ -28584,78 +28840,122 @@
       <c r="A203" s="4">
         <v>80000</v>
       </c>
-      <c r="B203" s="5"/>
-      <c r="C203" s="5"/>
+      <c r="B203" s="5">
+        <v>42</v>
+      </c>
+      <c r="C203" s="5">
+        <v>64</v>
+      </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" s="4">
         <v>90000</v>
       </c>
-      <c r="B204" s="5"/>
-      <c r="C204" s="5"/>
+      <c r="B204" s="5">
+        <v>44</v>
+      </c>
+      <c r="C204" s="5">
+        <v>76</v>
+      </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" s="4">
         <v>95000</v>
       </c>
-      <c r="B205" s="5"/>
-      <c r="C205" s="5"/>
+      <c r="B205" s="5">
+        <v>44</v>
+      </c>
+      <c r="C205" s="5">
+        <v>76</v>
+      </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="4">
         <v>100000</v>
       </c>
-      <c r="B206" s="5"/>
-      <c r="C206" s="5"/>
+      <c r="B206" s="5">
+        <v>44</v>
+      </c>
+      <c r="C206" s="5">
+        <v>76</v>
+      </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="4">
         <v>105000</v>
       </c>
-      <c r="B207" s="5"/>
-      <c r="C207" s="5"/>
+      <c r="B207" s="5">
+        <v>45</v>
+      </c>
+      <c r="C207" s="5">
+        <v>78</v>
+      </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="4">
         <v>110000</v>
       </c>
-      <c r="B208" s="5"/>
-      <c r="C208" s="5"/>
+      <c r="B208" s="5">
+        <v>51</v>
+      </c>
+      <c r="C208" s="5">
+        <v>84</v>
+      </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" s="6">
         <v>115000</v>
       </c>
-      <c r="B209" s="7"/>
-      <c r="C209" s="7"/>
+      <c r="B209" s="7">
+        <v>52</v>
+      </c>
+      <c r="C209" s="7">
+        <v>90</v>
+      </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" s="8">
         <v>120000</v>
       </c>
-      <c r="B210" s="5"/>
-      <c r="C210" s="5"/>
+      <c r="B210" s="5">
+        <v>52</v>
+      </c>
+      <c r="C210" s="5">
+        <v>92</v>
+      </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" s="4">
         <v>125000</v>
       </c>
-      <c r="B211" s="5"/>
-      <c r="C211" s="5"/>
+      <c r="B211" s="5">
+        <v>55</v>
+      </c>
+      <c r="C211" s="5">
+        <v>113</v>
+      </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" s="4">
         <v>130000</v>
       </c>
-      <c r="B212" s="5"/>
-      <c r="C212" s="5"/>
+      <c r="B212" s="5">
+        <v>56</v>
+      </c>
+      <c r="C212" s="5">
+        <v>115</v>
+      </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" s="4">
         <v>140000</v>
       </c>
-      <c r="B213" s="5"/>
-      <c r="C213" s="5"/>
+      <c r="B213" s="5">
+        <v>65</v>
+      </c>
+      <c r="C213" s="5">
+        <v>123</v>
+      </c>
     </row>
     <row r="214" spans="1:3">
       <c r="B214" t="s">
@@ -28677,78 +28977,122 @@
       <c r="A216" s="4">
         <v>80000</v>
       </c>
-      <c r="B216" s="5"/>
-      <c r="C216" s="5"/>
+      <c r="B216" s="5">
+        <v>37</v>
+      </c>
+      <c r="C216" s="5">
+        <v>55</v>
+      </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" s="4">
         <v>90000</v>
       </c>
-      <c r="B217" s="5"/>
-      <c r="C217" s="5"/>
+      <c r="B217" s="5">
+        <v>40</v>
+      </c>
+      <c r="C217" s="5">
+        <v>65</v>
+      </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="4">
         <v>95000</v>
       </c>
-      <c r="B218" s="5"/>
-      <c r="C218" s="5"/>
+      <c r="B218" s="5">
+        <v>43</v>
+      </c>
+      <c r="C218" s="5">
+        <v>69</v>
+      </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" s="4">
         <v>100000</v>
       </c>
-      <c r="B219" s="5"/>
-      <c r="C219" s="5"/>
+      <c r="B219" s="5">
+        <v>43</v>
+      </c>
+      <c r="C219" s="5">
+        <v>80</v>
+      </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" s="4">
         <v>105000</v>
       </c>
-      <c r="B220" s="5"/>
-      <c r="C220" s="5"/>
+      <c r="B220" s="5">
+        <v>46</v>
+      </c>
+      <c r="C220" s="5">
+        <v>83</v>
+      </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="4">
         <v>110000</v>
       </c>
-      <c r="B221" s="5"/>
-      <c r="C221" s="5"/>
+      <c r="B221" s="5">
+        <v>49</v>
+      </c>
+      <c r="C221" s="5">
+        <v>102</v>
+      </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="6">
         <v>115000</v>
       </c>
-      <c r="B222" s="7"/>
-      <c r="C222" s="7"/>
+      <c r="B222" s="7">
+        <v>51</v>
+      </c>
+      <c r="C222" s="7">
+        <v>102</v>
+      </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" s="8">
         <v>120000</v>
       </c>
-      <c r="B223" s="5"/>
-      <c r="C223" s="5"/>
+      <c r="B223" s="5">
+        <v>51</v>
+      </c>
+      <c r="C223" s="5">
+        <v>110</v>
+      </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" s="4">
         <v>125000</v>
       </c>
-      <c r="B224" s="5"/>
-      <c r="C224" s="5"/>
+      <c r="B224" s="5">
+        <v>52</v>
+      </c>
+      <c r="C224" s="5">
+        <v>112</v>
+      </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="4">
         <v>130000</v>
       </c>
-      <c r="B225" s="5"/>
-      <c r="C225" s="5"/>
+      <c r="B225" s="5">
+        <v>68</v>
+      </c>
+      <c r="C225" s="5">
+        <v>126</v>
+      </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="4">
         <v>140000</v>
       </c>
-      <c r="B226" s="5"/>
-      <c r="C226" s="5"/>
+      <c r="B226" s="5">
+        <v>80</v>
+      </c>
+      <c r="C226" s="5">
+        <v>219</v>
+      </c>
     </row>
     <row r="227" spans="1:3">
       <c r="B227" t="s">
@@ -28770,78 +29114,122 @@
       <c r="A229" s="4">
         <v>80000</v>
       </c>
-      <c r="B229" s="5"/>
-      <c r="C229" s="5"/>
+      <c r="B229" s="5">
+        <v>28</v>
+      </c>
+      <c r="C229" s="5">
+        <v>37</v>
+      </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="4">
         <v>90000</v>
       </c>
-      <c r="B230" s="5"/>
-      <c r="C230" s="5"/>
+      <c r="B230" s="5">
+        <v>33</v>
+      </c>
+      <c r="C230" s="5">
+        <v>45</v>
+      </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" s="4">
         <v>95000</v>
       </c>
-      <c r="B231" s="5"/>
-      <c r="C231" s="5"/>
+      <c r="B231" s="5">
+        <v>34</v>
+      </c>
+      <c r="C231" s="5">
+        <v>55</v>
+      </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" s="4">
         <v>100000</v>
       </c>
-      <c r="B232" s="5"/>
-      <c r="C232" s="5"/>
+      <c r="B232" s="5">
+        <v>36</v>
+      </c>
+      <c r="C232" s="5">
+        <v>57</v>
+      </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" s="4">
         <v>105000</v>
       </c>
-      <c r="B233" s="5"/>
-      <c r="C233" s="5"/>
+      <c r="B233" s="5">
+        <v>37</v>
+      </c>
+      <c r="C233" s="5">
+        <v>57</v>
+      </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" s="4">
         <v>110000</v>
       </c>
-      <c r="B234" s="5"/>
-      <c r="C234" s="5"/>
+      <c r="B234" s="5">
+        <v>37</v>
+      </c>
+      <c r="C234" s="5">
+        <v>59</v>
+      </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" s="6">
         <v>115000</v>
       </c>
-      <c r="B235" s="7"/>
-      <c r="C235" s="7"/>
+      <c r="B235" s="7">
+        <v>40</v>
+      </c>
+      <c r="C235" s="7">
+        <v>60</v>
+      </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="8">
         <v>120000</v>
       </c>
-      <c r="B236" s="5"/>
-      <c r="C236" s="5"/>
+      <c r="B236" s="5">
+        <v>46</v>
+      </c>
+      <c r="C236" s="5">
+        <v>74</v>
+      </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="4">
         <v>125000</v>
       </c>
-      <c r="B237" s="5"/>
-      <c r="C237" s="5"/>
+      <c r="B237" s="5">
+        <v>48</v>
+      </c>
+      <c r="C237" s="5">
+        <v>81</v>
+      </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="4">
         <v>130000</v>
       </c>
-      <c r="B238" s="5"/>
-      <c r="C238" s="5"/>
+      <c r="B238" s="5">
+        <v>51</v>
+      </c>
+      <c r="C238" s="5">
+        <v>83</v>
+      </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" s="4">
         <v>140000</v>
       </c>
-      <c r="B239" s="5"/>
-      <c r="C239" s="5"/>
+      <c r="B239" s="5">
+        <v>58</v>
+      </c>
+      <c r="C239" s="5">
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -28857,8 +29245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C285"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -28881,7 +29269,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="9">
-        <v>551</v>
+        <v>556</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -28890,7 +29278,7 @@
       </c>
       <c r="B3" s="9">
         <f>B1*B2*0.001</f>
-        <v>3.3611000000000005E-3</v>
+        <v>3.3916000000000003E-3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -28928,78 +29316,122 @@
       <c r="A9" s="4">
         <v>90000</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="5">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4">
         <v>100000</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="B10" s="5">
+        <v>25</v>
+      </c>
+      <c r="C10" s="5">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4">
         <v>105000</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="B11" s="5">
+        <v>27</v>
+      </c>
+      <c r="C11" s="5">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4">
         <v>110000</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="B12" s="5">
+        <v>30</v>
+      </c>
+      <c r="C12" s="5">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4">
         <v>115000</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="5">
+        <v>31</v>
+      </c>
+      <c r="C13" s="5">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="6">
         <v>120000</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="7">
+        <v>31</v>
+      </c>
+      <c r="C14" s="7">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="8">
         <v>125000</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="B15" s="5">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="4">
         <v>130000</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="B16" s="5">
+        <v>31</v>
+      </c>
+      <c r="C16" s="5">
+        <v>35</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="4">
         <v>140000</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="B17" s="5">
+        <v>31</v>
+      </c>
+      <c r="C17" s="5">
+        <v>35</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4">
         <v>150000</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="B18" s="5">
+        <v>33</v>
+      </c>
+      <c r="C18" s="5">
+        <v>36</v>
+      </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="4">
         <v>160000</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="B19" s="5">
+        <v>34</v>
+      </c>
+      <c r="C19" s="5">
+        <v>36</v>
+      </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" t="s">
@@ -29028,78 +29460,122 @@
       <c r="A23" s="4">
         <v>90000</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="B23" s="5">
+        <v>18</v>
+      </c>
+      <c r="C23" s="5">
+        <v>28</v>
+      </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="4">
         <v>100000</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="5">
+        <v>19</v>
+      </c>
+      <c r="C24" s="5">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="4">
         <v>105000</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="B25" s="5">
+        <v>20</v>
+      </c>
+      <c r="C25" s="5">
+        <v>31</v>
+      </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="4">
         <v>110000</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="B26" s="5">
+        <v>21</v>
+      </c>
+      <c r="C26" s="5">
+        <v>31</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="4">
         <v>115000</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="B27" s="5">
+        <v>21</v>
+      </c>
+      <c r="C27" s="5">
+        <v>31</v>
+      </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="6">
         <v>120000</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="B28" s="7">
+        <v>21</v>
+      </c>
+      <c r="C28" s="7">
+        <v>33</v>
+      </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="8">
         <v>125000</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+      <c r="B29" s="5">
+        <v>22</v>
+      </c>
+      <c r="C29" s="5">
+        <v>33</v>
+      </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="4">
         <v>130000</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="B30" s="5">
+        <v>22</v>
+      </c>
+      <c r="C30" s="5">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="4">
         <v>140000</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+      <c r="B31" s="5">
+        <v>25</v>
+      </c>
+      <c r="C31" s="5">
+        <v>36</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="4">
         <v>150000</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
+      <c r="B32" s="5">
+        <v>25</v>
+      </c>
+      <c r="C32" s="5">
+        <v>36</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="4">
         <v>160000</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="B33" s="5">
+        <v>28</v>
+      </c>
+      <c r="C33" s="5">
+        <v>36</v>
+      </c>
     </row>
     <row r="34" spans="1:3">
       <c r="B34" t="s">
@@ -29170,36 +29646,56 @@
       <c r="A43" s="8">
         <v>125000</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
+      <c r="B43" s="5">
+        <v>23</v>
+      </c>
+      <c r="C43" s="5">
+        <v>45</v>
+      </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="4">
         <v>130000</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
+      <c r="B44" s="5">
+        <v>24</v>
+      </c>
+      <c r="C44" s="5">
+        <v>45</v>
+      </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="4">
         <v>140000</v>
       </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
+      <c r="B45" s="5">
+        <v>25</v>
+      </c>
+      <c r="C45" s="5">
+        <v>46</v>
+      </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="4">
         <v>150000</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
+      <c r="B46" s="5">
+        <v>26</v>
+      </c>
+      <c r="C46" s="5">
+        <v>48</v>
+      </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="4">
         <v>160000</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
+      <c r="B47" s="5">
+        <v>26</v>
+      </c>
+      <c r="C47" s="5">
+        <v>48</v>
+      </c>
     </row>
     <row r="48" spans="1:3">
       <c r="B48" t="s">
@@ -29270,36 +29766,56 @@
       <c r="A57" s="8">
         <v>125000</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
+      <c r="B57" s="5">
+        <v>27</v>
+      </c>
+      <c r="C57" s="5">
+        <v>43</v>
+      </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="4">
         <v>130000</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
+      <c r="B58" s="5">
+        <v>27</v>
+      </c>
+      <c r="C58" s="5">
+        <v>43</v>
+      </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="4">
         <v>140000</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
+      <c r="B59" s="5">
+        <v>27</v>
+      </c>
+      <c r="C59" s="5">
+        <v>55</v>
+      </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="4">
         <v>150000</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
+      <c r="B60" s="5">
+        <v>35</v>
+      </c>
+      <c r="C60" s="5">
+        <v>55</v>
+      </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="4">
         <v>160000</v>
       </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
+      <c r="B61" s="5">
+        <v>36</v>
+      </c>
+      <c r="C61" s="5">
+        <v>57</v>
+      </c>
     </row>
     <row r="62" spans="1:3">
       <c r="B62" t="s">
@@ -29377,29 +29893,45 @@
       <c r="A72" s="4">
         <v>130000</v>
       </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
+      <c r="B72" s="5">
+        <v>20</v>
+      </c>
+      <c r="C72" s="5">
+        <v>42</v>
+      </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="4">
         <v>140000</v>
       </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
+      <c r="B73" s="5">
+        <v>21</v>
+      </c>
+      <c r="C73" s="5">
+        <v>42</v>
+      </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="4">
         <v>150000</v>
       </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
+      <c r="B74" s="5">
+        <v>23</v>
+      </c>
+      <c r="C74" s="5">
+        <v>44</v>
+      </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="4">
         <v>160000</v>
       </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
+      <c r="B75" s="5">
+        <v>24</v>
+      </c>
+      <c r="C75" s="5">
+        <v>45</v>
+      </c>
     </row>
     <row r="76" spans="1:3">
       <c r="B76" t="s">
@@ -29491,15 +30023,23 @@
       <c r="A88" s="4">
         <v>150000</v>
       </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
+      <c r="B88" s="5">
+        <v>55</v>
+      </c>
+      <c r="C88" s="5">
+        <v>145</v>
+      </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="4">
         <v>160000</v>
       </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
+      <c r="B89" s="5">
+        <v>58</v>
+      </c>
+      <c r="C89" s="5">
+        <v>148</v>
+      </c>
     </row>
     <row r="90" spans="1:3">
       <c r="B90" t="s">

</xml_diff>